<commit_message>
final edits before delivery week 1
</commit_message>
<xml_diff>
--- a/Week 1/gantt-chart_exam.xlsx
+++ b/Week 1/gantt-chart_exam.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fda248c8888d899/front_end/exam/Noroff Exam 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fda248c8888d899/front_end/exam/Noroff Exam 1/Week 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="194" documentId="8_{92D11D94-7E0C-4D48-8505-F2B714C11C86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E8F4E9DF-E481-8C49-BA29-52B22F97D006}"/>
+  <xr:revisionPtr revIDLastSave="202" documentId="8_{92D11D94-7E0C-4D48-8505-F2B714C11C86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{564B8AA3-B833-D143-A1D3-891C1E2922C9}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="1440" windowWidth="36740" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="150">
   <si>
     <t>Input Cell</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Creating Task Dependencies</t>
-  </si>
-  <si>
-    <t>[Task]</t>
   </si>
   <si>
     <t>Changing the Color of the Bars in the Gantt Chart</t>
@@ -2225,6 +2222,24 @@
     <xf numFmtId="0" fontId="38" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2232,27 +2247,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="41" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="41" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3085,11 +3082,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CA48"/>
+  <dimension ref="A1:CA35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3109,7 +3106,7 @@
   <sheetData>
     <row r="1" spans="1:79" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="78" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -3117,31 +3114,31 @@
       <c r="E1" s="43"/>
       <c r="F1" s="43"/>
       <c r="I1" s="82"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="117"/>
-      <c r="V1" s="117"/>
-      <c r="W1" s="117"/>
-      <c r="X1" s="117"/>
-      <c r="Y1" s="117"/>
-      <c r="Z1" s="117"/>
-      <c r="AA1" s="117"/>
-      <c r="AB1" s="117"/>
-      <c r="AC1" s="117"/>
-      <c r="AD1" s="117"/>
-      <c r="AE1" s="117"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="123"/>
+      <c r="M1" s="123"/>
+      <c r="N1" s="123"/>
+      <c r="O1" s="123"/>
+      <c r="P1" s="123"/>
+      <c r="Q1" s="123"/>
+      <c r="R1" s="123"/>
+      <c r="S1" s="123"/>
+      <c r="T1" s="123"/>
+      <c r="U1" s="123"/>
+      <c r="V1" s="123"/>
+      <c r="W1" s="123"/>
+      <c r="X1" s="123"/>
+      <c r="Y1" s="123"/>
+      <c r="Z1" s="123"/>
+      <c r="AA1" s="123"/>
+      <c r="AB1" s="123"/>
+      <c r="AC1" s="123"/>
+      <c r="AD1" s="123"/>
+      <c r="AE1" s="123"/>
     </row>
     <row r="2" spans="1:79" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -3180,198 +3177,198 @@
     <row r="4" spans="1:79" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="72"/>
       <c r="B4" s="76" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="122">
+        <v>60</v>
+      </c>
+      <c r="C4" s="125">
         <v>43941</v>
       </c>
-      <c r="D4" s="122"/>
-      <c r="E4" s="122"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="125"/>
       <c r="F4" s="73"/>
       <c r="G4" s="76" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" s="81">
         <v>1</v>
       </c>
       <c r="I4" s="74"/>
       <c r="J4" s="46"/>
-      <c r="K4" s="119" t="str">
+      <c r="K4" s="117" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="120"/>
-      <c r="M4" s="120"/>
-      <c r="N4" s="120"/>
-      <c r="O4" s="120"/>
-      <c r="P4" s="120"/>
-      <c r="Q4" s="121"/>
-      <c r="R4" s="119" t="str">
+      <c r="L4" s="118"/>
+      <c r="M4" s="118"/>
+      <c r="N4" s="118"/>
+      <c r="O4" s="118"/>
+      <c r="P4" s="118"/>
+      <c r="Q4" s="119"/>
+      <c r="R4" s="117" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="120"/>
-      <c r="T4" s="120"/>
-      <c r="U4" s="120"/>
-      <c r="V4" s="120"/>
-      <c r="W4" s="120"/>
-      <c r="X4" s="121"/>
-      <c r="Y4" s="119" t="str">
+      <c r="S4" s="118"/>
+      <c r="T4" s="118"/>
+      <c r="U4" s="118"/>
+      <c r="V4" s="118"/>
+      <c r="W4" s="118"/>
+      <c r="X4" s="119"/>
+      <c r="Y4" s="117" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="120"/>
-      <c r="AA4" s="120"/>
-      <c r="AB4" s="120"/>
-      <c r="AC4" s="120"/>
-      <c r="AD4" s="120"/>
-      <c r="AE4" s="121"/>
-      <c r="AF4" s="119" t="str">
+      <c r="Z4" s="118"/>
+      <c r="AA4" s="118"/>
+      <c r="AB4" s="118"/>
+      <c r="AC4" s="118"/>
+      <c r="AD4" s="118"/>
+      <c r="AE4" s="119"/>
+      <c r="AF4" s="117" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="120"/>
-      <c r="AH4" s="120"/>
-      <c r="AI4" s="120"/>
-      <c r="AJ4" s="120"/>
-      <c r="AK4" s="120"/>
-      <c r="AL4" s="121"/>
-      <c r="AM4" s="119" t="str">
+      <c r="AG4" s="118"/>
+      <c r="AH4" s="118"/>
+      <c r="AI4" s="118"/>
+      <c r="AJ4" s="118"/>
+      <c r="AK4" s="118"/>
+      <c r="AL4" s="119"/>
+      <c r="AM4" s="117" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="120"/>
-      <c r="AO4" s="120"/>
-      <c r="AP4" s="120"/>
-      <c r="AQ4" s="120"/>
-      <c r="AR4" s="120"/>
-      <c r="AS4" s="121"/>
-      <c r="AT4" s="119" t="str">
+      <c r="AN4" s="118"/>
+      <c r="AO4" s="118"/>
+      <c r="AP4" s="118"/>
+      <c r="AQ4" s="118"/>
+      <c r="AR4" s="118"/>
+      <c r="AS4" s="119"/>
+      <c r="AT4" s="117" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="120"/>
-      <c r="AV4" s="120"/>
-      <c r="AW4" s="120"/>
-      <c r="AX4" s="120"/>
-      <c r="AY4" s="120"/>
-      <c r="AZ4" s="121"/>
-      <c r="BA4" s="119" t="str">
+      <c r="AU4" s="118"/>
+      <c r="AV4" s="118"/>
+      <c r="AW4" s="118"/>
+      <c r="AX4" s="118"/>
+      <c r="AY4" s="118"/>
+      <c r="AZ4" s="119"/>
+      <c r="BA4" s="117" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="120"/>
-      <c r="BC4" s="120"/>
-      <c r="BD4" s="120"/>
-      <c r="BE4" s="120"/>
-      <c r="BF4" s="120"/>
-      <c r="BG4" s="121"/>
-      <c r="BH4" s="119" t="str">
+      <c r="BB4" s="118"/>
+      <c r="BC4" s="118"/>
+      <c r="BD4" s="118"/>
+      <c r="BE4" s="118"/>
+      <c r="BF4" s="118"/>
+      <c r="BG4" s="119"/>
+      <c r="BH4" s="117" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="120"/>
-      <c r="BJ4" s="120"/>
-      <c r="BK4" s="120"/>
-      <c r="BL4" s="120"/>
-      <c r="BM4" s="120"/>
-      <c r="BN4" s="121"/>
+      <c r="BI4" s="118"/>
+      <c r="BJ4" s="118"/>
+      <c r="BK4" s="118"/>
+      <c r="BL4" s="118"/>
+      <c r="BM4" s="118"/>
+      <c r="BN4" s="119"/>
     </row>
     <row r="5" spans="1:79" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="72"/>
       <c r="B5" s="76" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="118" t="s">
-        <v>126</v>
-      </c>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
+        <v>61</v>
+      </c>
+      <c r="C5" s="124" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="124"/>
+      <c r="E5" s="124"/>
       <c r="F5" s="75"/>
       <c r="G5" s="75"/>
       <c r="H5" s="75"/>
       <c r="I5" s="75"/>
       <c r="J5" s="46"/>
-      <c r="K5" s="123">
+      <c r="K5" s="120">
         <f>K6</f>
         <v>43941</v>
       </c>
-      <c r="L5" s="124"/>
-      <c r="M5" s="124"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="124"/>
-      <c r="P5" s="124"/>
-      <c r="Q5" s="125"/>
-      <c r="R5" s="123">
+      <c r="L5" s="121"/>
+      <c r="M5" s="121"/>
+      <c r="N5" s="121"/>
+      <c r="O5" s="121"/>
+      <c r="P5" s="121"/>
+      <c r="Q5" s="122"/>
+      <c r="R5" s="120">
         <f>R6</f>
         <v>43948</v>
       </c>
-      <c r="S5" s="124"/>
-      <c r="T5" s="124"/>
-      <c r="U5" s="124"/>
-      <c r="V5" s="124"/>
-      <c r="W5" s="124"/>
-      <c r="X5" s="125"/>
-      <c r="Y5" s="123">
+      <c r="S5" s="121"/>
+      <c r="T5" s="121"/>
+      <c r="U5" s="121"/>
+      <c r="V5" s="121"/>
+      <c r="W5" s="121"/>
+      <c r="X5" s="122"/>
+      <c r="Y5" s="120">
         <f>Y6</f>
         <v>43955</v>
       </c>
-      <c r="Z5" s="124"/>
-      <c r="AA5" s="124"/>
-      <c r="AB5" s="124"/>
-      <c r="AC5" s="124"/>
-      <c r="AD5" s="124"/>
-      <c r="AE5" s="125"/>
-      <c r="AF5" s="123">
+      <c r="Z5" s="121"/>
+      <c r="AA5" s="121"/>
+      <c r="AB5" s="121"/>
+      <c r="AC5" s="121"/>
+      <c r="AD5" s="121"/>
+      <c r="AE5" s="122"/>
+      <c r="AF5" s="120">
         <f>AF6</f>
         <v>43962</v>
       </c>
-      <c r="AG5" s="124"/>
-      <c r="AH5" s="124"/>
-      <c r="AI5" s="124"/>
-      <c r="AJ5" s="124"/>
-      <c r="AK5" s="124"/>
-      <c r="AL5" s="125"/>
-      <c r="AM5" s="123">
+      <c r="AG5" s="121"/>
+      <c r="AH5" s="121"/>
+      <c r="AI5" s="121"/>
+      <c r="AJ5" s="121"/>
+      <c r="AK5" s="121"/>
+      <c r="AL5" s="122"/>
+      <c r="AM5" s="120">
         <f>AM6</f>
         <v>43969</v>
       </c>
-      <c r="AN5" s="124"/>
-      <c r="AO5" s="124"/>
-      <c r="AP5" s="124"/>
-      <c r="AQ5" s="124"/>
-      <c r="AR5" s="124"/>
-      <c r="AS5" s="125"/>
-      <c r="AT5" s="123">
+      <c r="AN5" s="121"/>
+      <c r="AO5" s="121"/>
+      <c r="AP5" s="121"/>
+      <c r="AQ5" s="121"/>
+      <c r="AR5" s="121"/>
+      <c r="AS5" s="122"/>
+      <c r="AT5" s="120">
         <f>AT6</f>
         <v>43976</v>
       </c>
-      <c r="AU5" s="124"/>
-      <c r="AV5" s="124"/>
-      <c r="AW5" s="124"/>
-      <c r="AX5" s="124"/>
-      <c r="AY5" s="124"/>
-      <c r="AZ5" s="125"/>
-      <c r="BA5" s="123">
+      <c r="AU5" s="121"/>
+      <c r="AV5" s="121"/>
+      <c r="AW5" s="121"/>
+      <c r="AX5" s="121"/>
+      <c r="AY5" s="121"/>
+      <c r="AZ5" s="122"/>
+      <c r="BA5" s="120">
         <f>BA6</f>
         <v>43983</v>
       </c>
-      <c r="BB5" s="124"/>
-      <c r="BC5" s="124"/>
-      <c r="BD5" s="124"/>
-      <c r="BE5" s="124"/>
-      <c r="BF5" s="124"/>
-      <c r="BG5" s="125"/>
-      <c r="BH5" s="123">
+      <c r="BB5" s="121"/>
+      <c r="BC5" s="121"/>
+      <c r="BD5" s="121"/>
+      <c r="BE5" s="121"/>
+      <c r="BF5" s="121"/>
+      <c r="BG5" s="122"/>
+      <c r="BH5" s="120">
         <f>BH6</f>
         <v>43990</v>
       </c>
-      <c r="BI5" s="124"/>
-      <c r="BJ5" s="124"/>
-      <c r="BK5" s="124"/>
-      <c r="BL5" s="124"/>
-      <c r="BM5" s="124"/>
-      <c r="BN5" s="125"/>
+      <c r="BI5" s="121"/>
+      <c r="BJ5" s="121"/>
+      <c r="BK5" s="121"/>
+      <c r="BL5" s="121"/>
+      <c r="BM5" s="121"/>
+      <c r="BN5" s="122"/>
     </row>
     <row r="6" spans="1:79" x14ac:dyDescent="0.15">
       <c r="A6" s="45"/>
@@ -3379,13 +3376,13 @@
       <c r="C6" s="46"/>
       <c r="D6" s="47"/>
       <c r="E6" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="F6" s="46" t="s">
+      <c r="G6" s="46" t="s">
         <v>128</v>
-      </c>
-      <c r="G6" s="46" t="s">
-        <v>129</v>
       </c>
       <c r="H6" s="46"/>
       <c r="I6" s="46"/>
@@ -3621,7 +3618,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" s="58"/>
       <c r="D7" s="59"/>
@@ -3700,7 +3697,7 @@
         <v>1.1</v>
       </c>
       <c r="B8" s="79" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D8" s="80"/>
       <c r="E8" s="67">
@@ -3779,7 +3776,7 @@
         <v>1.2</v>
       </c>
       <c r="B9" s="79" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D9" s="80"/>
       <c r="E9" s="67">
@@ -3858,7 +3855,7 @@
         <v>1.3</v>
       </c>
       <c r="B10" s="79" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D10" s="80"/>
       <c r="E10" s="67">
@@ -3937,7 +3934,7 @@
         <v>1.4</v>
       </c>
       <c r="B11" s="79" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D11" s="80"/>
       <c r="E11" s="67">
@@ -4016,7 +4013,7 @@
         <v>1.5</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D12" s="80"/>
       <c r="E12" s="67">
@@ -4095,7 +4092,7 @@
         <v>1.6</v>
       </c>
       <c r="B13" s="79" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D13" s="80"/>
       <c r="E13" s="67">
@@ -4174,7 +4171,7 @@
         <v>1.7</v>
       </c>
       <c r="B14" s="79" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D14" s="80"/>
       <c r="E14" s="67">
@@ -4248,114 +4245,113 @@
       <c r="BN14" s="116"/>
     </row>
     <row r="15" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A15" s="50" t="str">
-        <f t="shared" ref="A15:A17" si="4">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>1.8</v>
-      </c>
-      <c r="B15" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="67">
-        <v>43941</v>
-      </c>
-      <c r="F15" s="68">
+      <c r="A15" s="56" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>2</v>
+      </c>
+      <c r="B15" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="77" t="str">
         <f>IF(ISBLANK(E15)," - ",IF(G15=0,E15,E15+G15-1))</f>
-        <v>43941</v>
-      </c>
-      <c r="G15" s="52">
-        <v>1</v>
-      </c>
-      <c r="H15" s="53"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="70"/>
-      <c r="L15" s="70"/>
-      <c r="M15" s="70"/>
-      <c r="N15" s="70"/>
-      <c r="O15" s="70"/>
-      <c r="P15" s="116"/>
-      <c r="Q15" s="116"/>
-      <c r="R15" s="70"/>
-      <c r="S15" s="70"/>
-      <c r="T15" s="70"/>
-      <c r="U15" s="70"/>
-      <c r="V15" s="70"/>
-      <c r="W15" s="116"/>
-      <c r="X15" s="116"/>
-      <c r="Y15" s="70"/>
-      <c r="Z15" s="70"/>
-      <c r="AA15" s="70"/>
-      <c r="AB15" s="70"/>
-      <c r="AC15" s="70"/>
-      <c r="AD15" s="116"/>
-      <c r="AE15" s="116"/>
-      <c r="AF15" s="70"/>
-      <c r="AG15" s="70"/>
-      <c r="AH15" s="70"/>
-      <c r="AI15" s="70"/>
-      <c r="AJ15" s="70"/>
-      <c r="AK15" s="116"/>
-      <c r="AL15" s="116"/>
-      <c r="AM15" s="70"/>
-      <c r="AN15" s="70"/>
-      <c r="AO15" s="70"/>
-      <c r="AP15" s="70"/>
-      <c r="AQ15" s="70"/>
-      <c r="AR15" s="116"/>
-      <c r="AS15" s="116"/>
-      <c r="AT15" s="70"/>
-      <c r="AU15" s="70"/>
-      <c r="AV15" s="70"/>
-      <c r="AW15" s="70"/>
-      <c r="AX15" s="70"/>
-      <c r="AY15" s="116"/>
-      <c r="AZ15" s="116"/>
-      <c r="BA15" s="70"/>
-      <c r="BB15" s="70"/>
-      <c r="BC15" s="70"/>
-      <c r="BD15" s="70"/>
-      <c r="BE15" s="70"/>
-      <c r="BF15" s="116"/>
-      <c r="BG15" s="116"/>
-      <c r="BH15" s="70"/>
-      <c r="BI15" s="70"/>
-      <c r="BJ15" s="70"/>
-      <c r="BK15" s="70"/>
-      <c r="BL15" s="70"/>
-      <c r="BM15" s="116"/>
-      <c r="BN15" s="116"/>
-      <c r="BO15" s="51"/>
-      <c r="BP15" s="51"/>
-      <c r="BQ15" s="51"/>
-      <c r="BR15" s="51"/>
-      <c r="BS15" s="51"/>
-      <c r="BT15" s="51"/>
-      <c r="BU15" s="51"/>
-      <c r="BV15" s="51"/>
-      <c r="BW15" s="51"/>
-      <c r="BX15" s="51"/>
-      <c r="BY15" s="51"/>
-      <c r="BZ15" s="51"/>
-      <c r="CA15" s="51"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G15" s="61"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="63" t="str">
+        <f>IF(OR(F15=0,E15=0)," - ",NETWORKDAYS(E15,F15))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J15" s="65"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="115"/>
+      <c r="Q15" s="115"/>
+      <c r="R15" s="69"/>
+      <c r="S15" s="69"/>
+      <c r="T15" s="69"/>
+      <c r="U15" s="69"/>
+      <c r="V15" s="69"/>
+      <c r="W15" s="115"/>
+      <c r="X15" s="115"/>
+      <c r="Y15" s="69"/>
+      <c r="Z15" s="69"/>
+      <c r="AA15" s="69"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="69"/>
+      <c r="AD15" s="115"/>
+      <c r="AE15" s="115"/>
+      <c r="AF15" s="69"/>
+      <c r="AG15" s="69"/>
+      <c r="AH15" s="69"/>
+      <c r="AI15" s="69"/>
+      <c r="AJ15" s="69"/>
+      <c r="AK15" s="115"/>
+      <c r="AL15" s="115"/>
+      <c r="AM15" s="69"/>
+      <c r="AN15" s="69"/>
+      <c r="AO15" s="69"/>
+      <c r="AP15" s="69"/>
+      <c r="AQ15" s="69"/>
+      <c r="AR15" s="115"/>
+      <c r="AS15" s="115"/>
+      <c r="AT15" s="69"/>
+      <c r="AU15" s="69"/>
+      <c r="AV15" s="69"/>
+      <c r="AW15" s="69"/>
+      <c r="AX15" s="69"/>
+      <c r="AY15" s="115"/>
+      <c r="AZ15" s="115"/>
+      <c r="BA15" s="69"/>
+      <c r="BB15" s="69"/>
+      <c r="BC15" s="69"/>
+      <c r="BD15" s="69"/>
+      <c r="BE15" s="69"/>
+      <c r="BF15" s="115"/>
+      <c r="BG15" s="115"/>
+      <c r="BH15" s="69"/>
+      <c r="BI15" s="69"/>
+      <c r="BJ15" s="69"/>
+      <c r="BK15" s="69"/>
+      <c r="BL15" s="69"/>
+      <c r="BM15" s="115"/>
+      <c r="BN15" s="115"/>
+      <c r="BO15" s="49"/>
+      <c r="BP15" s="49"/>
+      <c r="BQ15" s="49"/>
+      <c r="BR15" s="49"/>
+      <c r="BS15" s="49"/>
+      <c r="BT15" s="49"/>
+      <c r="BU15" s="49"/>
+      <c r="BV15" s="49"/>
+      <c r="BW15" s="49"/>
+      <c r="BX15" s="49"/>
+      <c r="BY15" s="49"/>
+      <c r="BZ15" s="49"/>
+      <c r="CA15" s="49"/>
     </row>
     <row r="16" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A16" s="50" t="str">
-        <f t="shared" si="4"/>
-        <v>1.9</v>
+        <f t="shared" ref="A16:A35" si="4">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>2.1</v>
       </c>
       <c r="B16" s="79" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="C16" s="51"/>
       <c r="D16" s="80"/>
       <c r="E16" s="67">
-        <v>43941</v>
+        <v>43948</v>
       </c>
       <c r="F16" s="68">
-        <f t="shared" ref="F16:F17" si="5">IF(ISBLANK(E16)," - ",IF(G16=0,E16,E16+G16-1))</f>
-        <v>43941</v>
+        <f>IF(ISBLANK(E16)," - ",IF(G16=0,E16,E16+G16-1))</f>
+        <v>43948</v>
       </c>
       <c r="G16" s="52">
         <v>1</v>
@@ -4436,19 +4432,19 @@
     <row r="17" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A17" s="50" t="str">
         <f t="shared" si="4"/>
-        <v>1.10</v>
+        <v>2.2</v>
       </c>
       <c r="B17" s="79" t="s">
-        <v>6</v>
+        <v>139</v>
       </c>
       <c r="C17" s="51"/>
       <c r="D17" s="80"/>
       <c r="E17" s="67">
-        <v>43941</v>
+        <v>43949</v>
       </c>
       <c r="F17" s="68">
-        <f t="shared" si="5"/>
-        <v>43941</v>
+        <f t="shared" ref="F17:F20" si="5">IF(ISBLANK(E17)," - ",IF(G17=0,E17,E17+G17-1))</f>
+        <v>43949</v>
       </c>
       <c r="G17" s="52">
         <v>1</v>
@@ -4458,7 +4454,7 @@
       <c r="J17" s="66"/>
       <c r="K17" s="70"/>
       <c r="L17" s="70"/>
-      <c r="M17" s="71"/>
+      <c r="M17" s="70"/>
       <c r="N17" s="70"/>
       <c r="O17" s="70"/>
       <c r="P17" s="116"/>
@@ -4527,113 +4523,114 @@
       <c r="CA17" s="51"/>
     </row>
     <row r="18" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A18" s="56" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+      <c r="A18" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v>2.3</v>
+      </c>
+      <c r="B18" s="79" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" s="51"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="67">
+        <v>43950</v>
+      </c>
+      <c r="F18" s="68">
+        <f t="shared" si="5"/>
+        <v>43951</v>
+      </c>
+      <c r="G18" s="52">
         <v>2</v>
       </c>
-      <c r="B18" s="57" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="77" t="str">
-        <f>IF(ISBLANK(E18)," - ",IF(G18=0,E18,E18+G18-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G18" s="61"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="63" t="str">
-        <f>IF(OR(F18=0,E18=0)," - ",NETWORKDAYS(E18,F18))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J18" s="65"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="69"/>
-      <c r="O18" s="69"/>
-      <c r="P18" s="115"/>
-      <c r="Q18" s="115"/>
-      <c r="R18" s="69"/>
-      <c r="S18" s="69"/>
-      <c r="T18" s="69"/>
-      <c r="U18" s="69"/>
-      <c r="V18" s="69"/>
-      <c r="W18" s="115"/>
-      <c r="X18" s="115"/>
-      <c r="Y18" s="69"/>
-      <c r="Z18" s="69"/>
-      <c r="AA18" s="69"/>
-      <c r="AB18" s="69"/>
-      <c r="AC18" s="69"/>
-      <c r="AD18" s="115"/>
-      <c r="AE18" s="115"/>
-      <c r="AF18" s="69"/>
-      <c r="AG18" s="69"/>
-      <c r="AH18" s="69"/>
-      <c r="AI18" s="69"/>
-      <c r="AJ18" s="69"/>
-      <c r="AK18" s="115"/>
-      <c r="AL18" s="115"/>
-      <c r="AM18" s="69"/>
-      <c r="AN18" s="69"/>
-      <c r="AO18" s="69"/>
-      <c r="AP18" s="69"/>
-      <c r="AQ18" s="69"/>
-      <c r="AR18" s="115"/>
-      <c r="AS18" s="115"/>
-      <c r="AT18" s="69"/>
-      <c r="AU18" s="69"/>
-      <c r="AV18" s="69"/>
-      <c r="AW18" s="69"/>
-      <c r="AX18" s="69"/>
-      <c r="AY18" s="115"/>
-      <c r="AZ18" s="115"/>
-      <c r="BA18" s="69"/>
-      <c r="BB18" s="69"/>
-      <c r="BC18" s="69"/>
-      <c r="BD18" s="69"/>
-      <c r="BE18" s="69"/>
-      <c r="BF18" s="115"/>
-      <c r="BG18" s="115"/>
-      <c r="BH18" s="69"/>
-      <c r="BI18" s="69"/>
-      <c r="BJ18" s="69"/>
-      <c r="BK18" s="69"/>
-      <c r="BL18" s="69"/>
-      <c r="BM18" s="115"/>
-      <c r="BN18" s="115"/>
-      <c r="BO18" s="49"/>
-      <c r="BP18" s="49"/>
-      <c r="BQ18" s="49"/>
-      <c r="BR18" s="49"/>
-      <c r="BS18" s="49"/>
-      <c r="BT18" s="49"/>
-      <c r="BU18" s="49"/>
-      <c r="BV18" s="49"/>
-      <c r="BW18" s="49"/>
-      <c r="BX18" s="49"/>
-      <c r="BY18" s="49"/>
-      <c r="BZ18" s="49"/>
-      <c r="CA18" s="49"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="71"/>
+      <c r="N18" s="70"/>
+      <c r="O18" s="70"/>
+      <c r="P18" s="116"/>
+      <c r="Q18" s="116"/>
+      <c r="R18" s="70"/>
+      <c r="S18" s="70"/>
+      <c r="T18" s="70"/>
+      <c r="U18" s="70"/>
+      <c r="V18" s="70"/>
+      <c r="W18" s="116"/>
+      <c r="X18" s="116"/>
+      <c r="Y18" s="70"/>
+      <c r="Z18" s="70"/>
+      <c r="AA18" s="70"/>
+      <c r="AB18" s="70"/>
+      <c r="AC18" s="70"/>
+      <c r="AD18" s="116"/>
+      <c r="AE18" s="116"/>
+      <c r="AF18" s="70"/>
+      <c r="AG18" s="70"/>
+      <c r="AH18" s="70"/>
+      <c r="AI18" s="70"/>
+      <c r="AJ18" s="70"/>
+      <c r="AK18" s="116"/>
+      <c r="AL18" s="116"/>
+      <c r="AM18" s="70"/>
+      <c r="AN18" s="70"/>
+      <c r="AO18" s="70"/>
+      <c r="AP18" s="70"/>
+      <c r="AQ18" s="70"/>
+      <c r="AR18" s="116"/>
+      <c r="AS18" s="116"/>
+      <c r="AT18" s="70"/>
+      <c r="AU18" s="70"/>
+      <c r="AV18" s="70"/>
+      <c r="AW18" s="70"/>
+      <c r="AX18" s="70"/>
+      <c r="AY18" s="116"/>
+      <c r="AZ18" s="116"/>
+      <c r="BA18" s="70"/>
+      <c r="BB18" s="70"/>
+      <c r="BC18" s="70"/>
+      <c r="BD18" s="70"/>
+      <c r="BE18" s="70"/>
+      <c r="BF18" s="116"/>
+      <c r="BG18" s="116"/>
+      <c r="BH18" s="70"/>
+      <c r="BI18" s="70"/>
+      <c r="BJ18" s="70"/>
+      <c r="BK18" s="70"/>
+      <c r="BL18" s="70"/>
+      <c r="BM18" s="116"/>
+      <c r="BN18" s="116"/>
+      <c r="BO18" s="51"/>
+      <c r="BP18" s="51"/>
+      <c r="BQ18" s="51"/>
+      <c r="BR18" s="51"/>
+      <c r="BS18" s="51"/>
+      <c r="BT18" s="51"/>
+      <c r="BU18" s="51"/>
+      <c r="BV18" s="51"/>
+      <c r="BW18" s="51"/>
+      <c r="BX18" s="51"/>
+      <c r="BY18" s="51"/>
+      <c r="BZ18" s="51"/>
+      <c r="CA18" s="51"/>
     </row>
     <row r="19" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A19" s="50" t="str">
-        <f t="shared" ref="A19:A46" si="6">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>2.1</v>
+        <f t="shared" si="4"/>
+        <v>2.4</v>
       </c>
       <c r="B19" s="79" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C19" s="51"/>
       <c r="D19" s="80"/>
       <c r="E19" s="67">
-        <v>43948</v>
+        <v>43952</v>
       </c>
       <c r="F19" s="68">
-        <f>IF(ISBLANK(E19)," - ",IF(G19=0,E19,E19+G19-1))</f>
-        <v>43948</v>
+        <f t="shared" si="5"/>
+        <v>43952</v>
       </c>
       <c r="G19" s="52">
         <v>1</v>
@@ -4713,23 +4710,23 @@
     </row>
     <row r="20" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A20" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>2.2</v>
+        <f t="shared" si="4"/>
+        <v>2.5</v>
       </c>
       <c r="B20" s="79" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C20" s="51"/>
       <c r="D20" s="80"/>
       <c r="E20" s="67">
-        <v>43949</v>
+        <v>43948</v>
       </c>
       <c r="F20" s="68">
-        <f t="shared" ref="F20:F25" si="7">IF(ISBLANK(E20)," - ",IF(G20=0,E20,E20+G20-1))</f>
-        <v>43949</v>
+        <f t="shared" si="5"/>
+        <v>43952</v>
       </c>
       <c r="G20" s="52">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H20" s="53"/>
       <c r="I20" s="54"/>
@@ -4805,117 +4802,116 @@
       <c r="CA20" s="51"/>
     </row>
     <row r="21" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A21" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>2.3</v>
-      </c>
-      <c r="B21" s="79" t="s">
-        <v>141</v>
-      </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="67">
-        <v>43950</v>
-      </c>
-      <c r="F21" s="68">
-        <f t="shared" si="7"/>
-        <v>43951</v>
-      </c>
-      <c r="G21" s="52">
-        <v>2</v>
-      </c>
-      <c r="H21" s="53"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="66"/>
-      <c r="K21" s="70"/>
-      <c r="L21" s="70"/>
-      <c r="M21" s="71"/>
-      <c r="N21" s="70"/>
-      <c r="O21" s="70"/>
-      <c r="P21" s="116"/>
-      <c r="Q21" s="116"/>
-      <c r="R21" s="70"/>
-      <c r="S21" s="70"/>
-      <c r="T21" s="70"/>
-      <c r="U21" s="70"/>
-      <c r="V21" s="70"/>
-      <c r="W21" s="116"/>
-      <c r="X21" s="116"/>
-      <c r="Y21" s="70"/>
-      <c r="Z21" s="70"/>
-      <c r="AA21" s="70"/>
-      <c r="AB21" s="70"/>
-      <c r="AC21" s="70"/>
-      <c r="AD21" s="116"/>
-      <c r="AE21" s="116"/>
-      <c r="AF21" s="70"/>
-      <c r="AG21" s="70"/>
-      <c r="AH21" s="70"/>
-      <c r="AI21" s="70"/>
-      <c r="AJ21" s="70"/>
-      <c r="AK21" s="116"/>
-      <c r="AL21" s="116"/>
-      <c r="AM21" s="70"/>
-      <c r="AN21" s="70"/>
-      <c r="AO21" s="70"/>
-      <c r="AP21" s="70"/>
-      <c r="AQ21" s="70"/>
-      <c r="AR21" s="116"/>
-      <c r="AS21" s="116"/>
-      <c r="AT21" s="70"/>
-      <c r="AU21" s="70"/>
-      <c r="AV21" s="70"/>
-      <c r="AW21" s="70"/>
-      <c r="AX21" s="70"/>
-      <c r="AY21" s="116"/>
-      <c r="AZ21" s="116"/>
-      <c r="BA21" s="70"/>
-      <c r="BB21" s="70"/>
-      <c r="BC21" s="70"/>
-      <c r="BD21" s="70"/>
-      <c r="BE21" s="70"/>
-      <c r="BF21" s="116"/>
-      <c r="BG21" s="116"/>
-      <c r="BH21" s="70"/>
-      <c r="BI21" s="70"/>
-      <c r="BJ21" s="70"/>
-      <c r="BK21" s="70"/>
-      <c r="BL21" s="70"/>
-      <c r="BM21" s="116"/>
-      <c r="BN21" s="116"/>
-      <c r="BO21" s="51"/>
-      <c r="BP21" s="51"/>
-      <c r="BQ21" s="51"/>
-      <c r="BR21" s="51"/>
-      <c r="BS21" s="51"/>
-      <c r="BT21" s="51"/>
-      <c r="BU21" s="51"/>
-      <c r="BV21" s="51"/>
-      <c r="BW21" s="51"/>
-      <c r="BX21" s="51"/>
-      <c r="BY21" s="51"/>
-      <c r="BZ21" s="51"/>
-      <c r="CA21" s="51"/>
+      <c r="A21" s="56" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>3</v>
+      </c>
+      <c r="B21" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="58"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="77" t="str">
+        <f>IF(ISBLANK(E21)," - ",IF(G21=0,E21,E21+G21-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G21" s="61"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="63" t="str">
+        <f>IF(OR(F21=0,E21=0)," - ",NETWORKDAYS(E21,F21))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J21" s="65"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="69"/>
+      <c r="N21" s="69"/>
+      <c r="O21" s="69"/>
+      <c r="P21" s="115"/>
+      <c r="Q21" s="115"/>
+      <c r="R21" s="69"/>
+      <c r="S21" s="69"/>
+      <c r="T21" s="69"/>
+      <c r="U21" s="69"/>
+      <c r="V21" s="69"/>
+      <c r="W21" s="115"/>
+      <c r="X21" s="115"/>
+      <c r="Y21" s="69"/>
+      <c r="Z21" s="69"/>
+      <c r="AA21" s="69"/>
+      <c r="AB21" s="69"/>
+      <c r="AC21" s="69"/>
+      <c r="AD21" s="115"/>
+      <c r="AE21" s="115"/>
+      <c r="AF21" s="69"/>
+      <c r="AG21" s="69"/>
+      <c r="AH21" s="69"/>
+      <c r="AI21" s="69"/>
+      <c r="AJ21" s="69"/>
+      <c r="AK21" s="115"/>
+      <c r="AL21" s="115"/>
+      <c r="AM21" s="69"/>
+      <c r="AN21" s="69"/>
+      <c r="AO21" s="69"/>
+      <c r="AP21" s="69"/>
+      <c r="AQ21" s="69"/>
+      <c r="AR21" s="115"/>
+      <c r="AS21" s="115"/>
+      <c r="AT21" s="69"/>
+      <c r="AU21" s="69"/>
+      <c r="AV21" s="69"/>
+      <c r="AW21" s="69"/>
+      <c r="AX21" s="69"/>
+      <c r="AY21" s="115"/>
+      <c r="AZ21" s="115"/>
+      <c r="BA21" s="69"/>
+      <c r="BB21" s="69"/>
+      <c r="BC21" s="69"/>
+      <c r="BD21" s="69"/>
+      <c r="BE21" s="69"/>
+      <c r="BF21" s="115"/>
+      <c r="BG21" s="115"/>
+      <c r="BH21" s="69"/>
+      <c r="BI21" s="69"/>
+      <c r="BJ21" s="69"/>
+      <c r="BK21" s="69"/>
+      <c r="BL21" s="69"/>
+      <c r="BM21" s="115"/>
+      <c r="BN21" s="115"/>
+      <c r="BO21" s="49"/>
+      <c r="BP21" s="49"/>
+      <c r="BQ21" s="49"/>
+      <c r="BR21" s="49"/>
+      <c r="BS21" s="49"/>
+      <c r="BT21" s="49"/>
+      <c r="BU21" s="49"/>
+      <c r="BV21" s="49"/>
+      <c r="BW21" s="49"/>
+      <c r="BX21" s="49"/>
+      <c r="BY21" s="49"/>
+      <c r="BZ21" s="49"/>
+      <c r="CA21" s="49"/>
     </row>
     <row r="22" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A22" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>2.4</v>
+        <f t="shared" si="4"/>
+        <v>3.1</v>
       </c>
       <c r="B22" s="79" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C22" s="51"/>
       <c r="D22" s="80"/>
       <c r="E22" s="67">
-        <v>43952</v>
+        <v>43955</v>
       </c>
       <c r="F22" s="68">
-        <f t="shared" si="7"/>
-        <v>43952</v>
+        <f>IF(ISBLANK(E22)," - ",IF(G22=0,E22,E22+G22-1))</f>
+        <v>43956</v>
       </c>
       <c r="G22" s="52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="53"/>
       <c r="I22" s="54"/>
@@ -4992,23 +4988,23 @@
     </row>
     <row r="23" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A23" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>2.5</v>
+        <f t="shared" si="4"/>
+        <v>3.2</v>
       </c>
       <c r="B23" s="79" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C23" s="51"/>
       <c r="D23" s="80"/>
       <c r="E23" s="67">
-        <v>43948</v>
+        <v>43957</v>
       </c>
       <c r="F23" s="68">
-        <f t="shared" si="7"/>
-        <v>43952</v>
+        <f t="shared" ref="F23:F25" si="6">IF(ISBLANK(E23)," - ",IF(G23=0,E23,E23+G23-1))</f>
+        <v>43959</v>
       </c>
       <c r="G23" s="52">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H23" s="53"/>
       <c r="I23" s="54"/>
@@ -5085,30 +5081,30 @@
     </row>
     <row r="24" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A24" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>2.6</v>
+        <f t="shared" si="4"/>
+        <v>3.3</v>
       </c>
       <c r="B24" s="79" t="s">
-        <v>6</v>
+        <v>142</v>
       </c>
       <c r="C24" s="51"/>
       <c r="D24" s="80"/>
       <c r="E24" s="67">
-        <v>43941</v>
+        <v>43958</v>
       </c>
       <c r="F24" s="68">
-        <f t="shared" si="7"/>
-        <v>43941</v>
+        <f t="shared" si="6"/>
+        <v>43959</v>
       </c>
       <c r="G24" s="52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24" s="53"/>
       <c r="I24" s="54"/>
       <c r="J24" s="66"/>
       <c r="K24" s="70"/>
       <c r="L24" s="70"/>
-      <c r="M24" s="70"/>
+      <c r="M24" s="71"/>
       <c r="N24" s="70"/>
       <c r="O24" s="70"/>
       <c r="P24" s="116"/>
@@ -5178,23 +5174,23 @@
     </row>
     <row r="25" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A25" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>2.7</v>
+        <f t="shared" si="4"/>
+        <v>3.4</v>
       </c>
       <c r="B25" s="79" t="s">
-        <v>6</v>
+        <v>134</v>
       </c>
       <c r="C25" s="51"/>
       <c r="D25" s="80"/>
       <c r="E25" s="67">
-        <v>43941</v>
+        <v>43955</v>
       </c>
       <c r="F25" s="68">
-        <f t="shared" si="7"/>
-        <v>43941</v>
+        <f t="shared" si="6"/>
+        <v>43959</v>
       </c>
       <c r="G25" s="52">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H25" s="53"/>
       <c r="I25" s="54"/>
@@ -5272,7 +5268,7 @@
     <row r="26" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A26" s="56" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B26" s="57" t="s">
         <v>123</v>
@@ -5363,23 +5359,23 @@
     </row>
     <row r="27" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A27" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>3.1</v>
+        <f t="shared" si="4"/>
+        <v>4.1</v>
       </c>
       <c r="B27" s="79" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C27" s="51"/>
       <c r="D27" s="80"/>
       <c r="E27" s="67">
-        <v>43955</v>
+        <v>43962</v>
       </c>
       <c r="F27" s="68">
         <f>IF(ISBLANK(E27)," - ",IF(G27=0,E27,E27+G27-1))</f>
-        <v>43956</v>
+        <v>43966</v>
       </c>
       <c r="G27" s="52">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H27" s="53"/>
       <c r="I27" s="54"/>
@@ -5456,8 +5452,8 @@
     </row>
     <row r="28" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A28" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>3.2</v>
+        <f t="shared" si="4"/>
+        <v>4.2</v>
       </c>
       <c r="B28" s="79" t="s">
         <v>142</v>
@@ -5465,14 +5461,14 @@
       <c r="C28" s="51"/>
       <c r="D28" s="80"/>
       <c r="E28" s="67">
-        <v>43957</v>
+        <v>43962</v>
       </c>
       <c r="F28" s="68">
-        <f t="shared" ref="F28:F32" si="8">IF(ISBLANK(E28)," - ",IF(G28=0,E28,E28+G28-1))</f>
-        <v>43959</v>
+        <f t="shared" ref="F28:F30" si="7">IF(ISBLANK(E28)," - ",IF(G28=0,E28,E28+G28-1))</f>
+        <v>43966</v>
       </c>
       <c r="G28" s="52">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H28" s="53"/>
       <c r="I28" s="54"/>
@@ -5549,8 +5545,8 @@
     </row>
     <row r="29" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A29" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>3.3</v>
+        <f t="shared" si="4"/>
+        <v>4.3</v>
       </c>
       <c r="B29" s="79" t="s">
         <v>143</v>
@@ -5558,14 +5554,14 @@
       <c r="C29" s="51"/>
       <c r="D29" s="80"/>
       <c r="E29" s="67">
-        <v>43958</v>
+        <v>43962</v>
       </c>
       <c r="F29" s="68">
-        <f t="shared" si="8"/>
-        <v>43959</v>
+        <f t="shared" si="7"/>
+        <v>43966</v>
       </c>
       <c r="G29" s="52">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H29" s="53"/>
       <c r="I29" s="54"/>
@@ -5642,20 +5638,20 @@
     </row>
     <row r="30" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A30" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>3.4</v>
+        <f t="shared" si="4"/>
+        <v>4.4</v>
       </c>
       <c r="B30" s="79" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C30" s="51"/>
       <c r="D30" s="80"/>
       <c r="E30" s="67">
-        <v>43955</v>
+        <v>43962</v>
       </c>
       <c r="F30" s="68">
-        <f t="shared" si="8"/>
-        <v>43959</v>
+        <f t="shared" si="7"/>
+        <v>43966</v>
       </c>
       <c r="G30" s="52">
         <v>5</v>
@@ -5734,117 +5730,116 @@
       <c r="CA30" s="51"/>
     </row>
     <row r="31" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A31" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>3.5</v>
-      </c>
-      <c r="B31" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="51"/>
-      <c r="D31" s="80"/>
-      <c r="E31" s="67">
-        <v>43941</v>
-      </c>
-      <c r="F31" s="68">
-        <f t="shared" si="8"/>
-        <v>43941</v>
-      </c>
-      <c r="G31" s="52">
-        <v>1</v>
-      </c>
-      <c r="H31" s="53"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="66"/>
-      <c r="K31" s="70"/>
-      <c r="L31" s="70"/>
-      <c r="M31" s="70"/>
-      <c r="N31" s="70"/>
-      <c r="O31" s="70"/>
-      <c r="P31" s="116"/>
-      <c r="Q31" s="116"/>
-      <c r="R31" s="70"/>
-      <c r="S31" s="70"/>
-      <c r="T31" s="70"/>
-      <c r="U31" s="70"/>
-      <c r="V31" s="70"/>
-      <c r="W31" s="116"/>
-      <c r="X31" s="116"/>
-      <c r="Y31" s="70"/>
-      <c r="Z31" s="70"/>
-      <c r="AA31" s="70"/>
-      <c r="AB31" s="70"/>
-      <c r="AC31" s="70"/>
-      <c r="AD31" s="116"/>
-      <c r="AE31" s="116"/>
-      <c r="AF31" s="70"/>
-      <c r="AG31" s="70"/>
-      <c r="AH31" s="70"/>
-      <c r="AI31" s="70"/>
-      <c r="AJ31" s="70"/>
-      <c r="AK31" s="116"/>
-      <c r="AL31" s="116"/>
-      <c r="AM31" s="70"/>
-      <c r="AN31" s="70"/>
-      <c r="AO31" s="70"/>
-      <c r="AP31" s="70"/>
-      <c r="AQ31" s="70"/>
-      <c r="AR31" s="116"/>
-      <c r="AS31" s="116"/>
-      <c r="AT31" s="70"/>
-      <c r="AU31" s="70"/>
-      <c r="AV31" s="70"/>
-      <c r="AW31" s="70"/>
-      <c r="AX31" s="70"/>
-      <c r="AY31" s="116"/>
-      <c r="AZ31" s="116"/>
-      <c r="BA31" s="70"/>
-      <c r="BB31" s="70"/>
-      <c r="BC31" s="70"/>
-      <c r="BD31" s="70"/>
-      <c r="BE31" s="70"/>
-      <c r="BF31" s="116"/>
-      <c r="BG31" s="116"/>
-      <c r="BH31" s="70"/>
-      <c r="BI31" s="70"/>
-      <c r="BJ31" s="70"/>
-      <c r="BK31" s="70"/>
-      <c r="BL31" s="70"/>
-      <c r="BM31" s="116"/>
-      <c r="BN31" s="116"/>
-      <c r="BO31" s="51"/>
-      <c r="BP31" s="51"/>
-      <c r="BQ31" s="51"/>
-      <c r="BR31" s="51"/>
-      <c r="BS31" s="51"/>
-      <c r="BT31" s="51"/>
-      <c r="BU31" s="51"/>
-      <c r="BV31" s="51"/>
-      <c r="BW31" s="51"/>
-      <c r="BX31" s="51"/>
-      <c r="BY31" s="51"/>
-      <c r="BZ31" s="51"/>
-      <c r="CA31" s="51"/>
+      <c r="A31" s="56" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>5</v>
+      </c>
+      <c r="B31" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="58"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="77" t="str">
+        <f>IF(ISBLANK(E31)," - ",IF(G31=0,E31,E31+G31-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G31" s="61"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="63" t="str">
+        <f>IF(OR(F31=0,E31=0)," - ",NETWORKDAYS(E31,F31))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J31" s="65"/>
+      <c r="K31" s="69"/>
+      <c r="L31" s="69"/>
+      <c r="M31" s="69"/>
+      <c r="N31" s="69"/>
+      <c r="O31" s="69"/>
+      <c r="P31" s="115"/>
+      <c r="Q31" s="115"/>
+      <c r="R31" s="69"/>
+      <c r="S31" s="69"/>
+      <c r="T31" s="69"/>
+      <c r="U31" s="69"/>
+      <c r="V31" s="69"/>
+      <c r="W31" s="115"/>
+      <c r="X31" s="115"/>
+      <c r="Y31" s="69"/>
+      <c r="Z31" s="69"/>
+      <c r="AA31" s="69"/>
+      <c r="AB31" s="69"/>
+      <c r="AC31" s="69"/>
+      <c r="AD31" s="115"/>
+      <c r="AE31" s="115"/>
+      <c r="AF31" s="69"/>
+      <c r="AG31" s="69"/>
+      <c r="AH31" s="69"/>
+      <c r="AI31" s="69"/>
+      <c r="AJ31" s="69"/>
+      <c r="AK31" s="115"/>
+      <c r="AL31" s="115"/>
+      <c r="AM31" s="69"/>
+      <c r="AN31" s="69"/>
+      <c r="AO31" s="69"/>
+      <c r="AP31" s="69"/>
+      <c r="AQ31" s="69"/>
+      <c r="AR31" s="115"/>
+      <c r="AS31" s="115"/>
+      <c r="AT31" s="69"/>
+      <c r="AU31" s="69"/>
+      <c r="AV31" s="69"/>
+      <c r="AW31" s="69"/>
+      <c r="AX31" s="69"/>
+      <c r="AY31" s="115"/>
+      <c r="AZ31" s="115"/>
+      <c r="BA31" s="69"/>
+      <c r="BB31" s="69"/>
+      <c r="BC31" s="69"/>
+      <c r="BD31" s="69"/>
+      <c r="BE31" s="69"/>
+      <c r="BF31" s="115"/>
+      <c r="BG31" s="115"/>
+      <c r="BH31" s="69"/>
+      <c r="BI31" s="69"/>
+      <c r="BJ31" s="69"/>
+      <c r="BK31" s="69"/>
+      <c r="BL31" s="69"/>
+      <c r="BM31" s="115"/>
+      <c r="BN31" s="115"/>
+      <c r="BO31" s="49"/>
+      <c r="BP31" s="49"/>
+      <c r="BQ31" s="49"/>
+      <c r="BR31" s="49"/>
+      <c r="BS31" s="49"/>
+      <c r="BT31" s="49"/>
+      <c r="BU31" s="49"/>
+      <c r="BV31" s="49"/>
+      <c r="BW31" s="49"/>
+      <c r="BX31" s="49"/>
+      <c r="BY31" s="49"/>
+      <c r="BZ31" s="49"/>
+      <c r="CA31" s="49"/>
     </row>
     <row r="32" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A32" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>3.6</v>
+        <f t="shared" si="4"/>
+        <v>5.1</v>
       </c>
       <c r="B32" s="79" t="s">
-        <v>6</v>
+        <v>147</v>
       </c>
       <c r="C32" s="51"/>
       <c r="D32" s="80"/>
       <c r="E32" s="67">
-        <v>43941</v>
+        <v>43969</v>
       </c>
       <c r="F32" s="68">
-        <f t="shared" si="8"/>
-        <v>43941</v>
+        <f>IF(ISBLANK(E32)," - ",IF(G32=0,E32,E32+G32-1))</f>
+        <v>43972</v>
       </c>
       <c r="G32" s="52">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H32" s="53"/>
       <c r="I32" s="54"/>
@@ -5920,123 +5915,124 @@
       <c r="CA32" s="51"/>
     </row>
     <row r="33" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A33" s="56" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+      <c r="A33" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v>5.2</v>
+      </c>
+      <c r="B33" s="79" t="s">
+        <v>144</v>
+      </c>
+      <c r="C33" s="51"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="67">
+        <v>43969</v>
+      </c>
+      <c r="F33" s="68">
+        <f t="shared" ref="F33:F35" si="8">IF(ISBLANK(E33)," - ",IF(G33=0,E33,E33+G33-1))</f>
+        <v>43972</v>
+      </c>
+      <c r="G33" s="52">
         <v>4</v>
       </c>
-      <c r="B33" s="57" t="s">
-        <v>124</v>
-      </c>
-      <c r="C33" s="58"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="77" t="str">
-        <f>IF(ISBLANK(E33)," - ",IF(G33=0,E33,E33+G33-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G33" s="61"/>
-      <c r="H33" s="62"/>
-      <c r="I33" s="63" t="str">
-        <f>IF(OR(F33=0,E33=0)," - ",NETWORKDAYS(E33,F33))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J33" s="65"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="69"/>
-      <c r="M33" s="69"/>
-      <c r="N33" s="69"/>
-      <c r="O33" s="69"/>
-      <c r="P33" s="115"/>
-      <c r="Q33" s="115"/>
-      <c r="R33" s="69"/>
-      <c r="S33" s="69"/>
-      <c r="T33" s="69"/>
-      <c r="U33" s="69"/>
-      <c r="V33" s="69"/>
-      <c r="W33" s="115"/>
-      <c r="X33" s="115"/>
-      <c r="Y33" s="69"/>
-      <c r="Z33" s="69"/>
-      <c r="AA33" s="69"/>
-      <c r="AB33" s="69"/>
-      <c r="AC33" s="69"/>
-      <c r="AD33" s="115"/>
-      <c r="AE33" s="115"/>
-      <c r="AF33" s="69"/>
-      <c r="AG33" s="69"/>
-      <c r="AH33" s="69"/>
-      <c r="AI33" s="69"/>
-      <c r="AJ33" s="69"/>
-      <c r="AK33" s="115"/>
-      <c r="AL33" s="115"/>
-      <c r="AM33" s="69"/>
-      <c r="AN33" s="69"/>
-      <c r="AO33" s="69"/>
-      <c r="AP33" s="69"/>
-      <c r="AQ33" s="69"/>
-      <c r="AR33" s="115"/>
-      <c r="AS33" s="115"/>
-      <c r="AT33" s="69"/>
-      <c r="AU33" s="69"/>
-      <c r="AV33" s="69"/>
-      <c r="AW33" s="69"/>
-      <c r="AX33" s="69"/>
-      <c r="AY33" s="115"/>
-      <c r="AZ33" s="115"/>
-      <c r="BA33" s="69"/>
-      <c r="BB33" s="69"/>
-      <c r="BC33" s="69"/>
-      <c r="BD33" s="69"/>
-      <c r="BE33" s="69"/>
-      <c r="BF33" s="115"/>
-      <c r="BG33" s="115"/>
-      <c r="BH33" s="69"/>
-      <c r="BI33" s="69"/>
-      <c r="BJ33" s="69"/>
-      <c r="BK33" s="69"/>
-      <c r="BL33" s="69"/>
-      <c r="BM33" s="115"/>
-      <c r="BN33" s="115"/>
-      <c r="BO33" s="49"/>
-      <c r="BP33" s="49"/>
-      <c r="BQ33" s="49"/>
-      <c r="BR33" s="49"/>
-      <c r="BS33" s="49"/>
-      <c r="BT33" s="49"/>
-      <c r="BU33" s="49"/>
-      <c r="BV33" s="49"/>
-      <c r="BW33" s="49"/>
-      <c r="BX33" s="49"/>
-      <c r="BY33" s="49"/>
-      <c r="BZ33" s="49"/>
-      <c r="CA33" s="49"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="66"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="70"/>
+      <c r="N33" s="70"/>
+      <c r="O33" s="70"/>
+      <c r="P33" s="116"/>
+      <c r="Q33" s="116"/>
+      <c r="R33" s="70"/>
+      <c r="S33" s="70"/>
+      <c r="T33" s="70"/>
+      <c r="U33" s="70"/>
+      <c r="V33" s="70"/>
+      <c r="W33" s="116"/>
+      <c r="X33" s="116"/>
+      <c r="Y33" s="70"/>
+      <c r="Z33" s="70"/>
+      <c r="AA33" s="70"/>
+      <c r="AB33" s="70"/>
+      <c r="AC33" s="70"/>
+      <c r="AD33" s="116"/>
+      <c r="AE33" s="116"/>
+      <c r="AF33" s="70"/>
+      <c r="AG33" s="70"/>
+      <c r="AH33" s="70"/>
+      <c r="AI33" s="70"/>
+      <c r="AJ33" s="70"/>
+      <c r="AK33" s="116"/>
+      <c r="AL33" s="116"/>
+      <c r="AM33" s="70"/>
+      <c r="AN33" s="70"/>
+      <c r="AO33" s="70"/>
+      <c r="AP33" s="70"/>
+      <c r="AQ33" s="70"/>
+      <c r="AR33" s="116"/>
+      <c r="AS33" s="116"/>
+      <c r="AT33" s="70"/>
+      <c r="AU33" s="70"/>
+      <c r="AV33" s="70"/>
+      <c r="AW33" s="70"/>
+      <c r="AX33" s="70"/>
+      <c r="AY33" s="116"/>
+      <c r="AZ33" s="116"/>
+      <c r="BA33" s="70"/>
+      <c r="BB33" s="70"/>
+      <c r="BC33" s="70"/>
+      <c r="BD33" s="70"/>
+      <c r="BE33" s="70"/>
+      <c r="BF33" s="116"/>
+      <c r="BG33" s="116"/>
+      <c r="BH33" s="70"/>
+      <c r="BI33" s="70"/>
+      <c r="BJ33" s="70"/>
+      <c r="BK33" s="70"/>
+      <c r="BL33" s="70"/>
+      <c r="BM33" s="116"/>
+      <c r="BN33" s="116"/>
+      <c r="BO33" s="51"/>
+      <c r="BP33" s="51"/>
+      <c r="BQ33" s="51"/>
+      <c r="BR33" s="51"/>
+      <c r="BS33" s="51"/>
+      <c r="BT33" s="51"/>
+      <c r="BU33" s="51"/>
+      <c r="BV33" s="51"/>
+      <c r="BW33" s="51"/>
+      <c r="BX33" s="51"/>
+      <c r="BY33" s="51"/>
+      <c r="BZ33" s="51"/>
+      <c r="CA33" s="51"/>
     </row>
     <row r="34" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A34" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>4.1</v>
+        <f t="shared" si="4"/>
+        <v>5.3</v>
       </c>
       <c r="B34" s="79" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C34" s="51"/>
       <c r="D34" s="80"/>
       <c r="E34" s="67">
-        <v>43962</v>
+        <v>43972</v>
       </c>
       <c r="F34" s="68">
-        <f>IF(ISBLANK(E34)," - ",IF(G34=0,E34,E34+G34-1))</f>
-        <v>43966</v>
+        <f t="shared" si="8"/>
+        <v>43973</v>
       </c>
       <c r="G34" s="52">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H34" s="53"/>
       <c r="I34" s="54"/>
       <c r="J34" s="66"/>
       <c r="K34" s="70"/>
       <c r="L34" s="70"/>
-      <c r="M34" s="70"/>
+      <c r="M34" s="71"/>
       <c r="N34" s="70"/>
       <c r="O34" s="70"/>
       <c r="P34" s="116"/>
@@ -6106,23 +6102,23 @@
     </row>
     <row r="35" spans="1:79" ht="18" x14ac:dyDescent="0.15">
       <c r="A35" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>4.2</v>
+        <f t="shared" si="4"/>
+        <v>5.4</v>
       </c>
       <c r="B35" s="79" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C35" s="51"/>
       <c r="D35" s="80"/>
       <c r="E35" s="67">
-        <v>43962</v>
+        <v>43973</v>
       </c>
       <c r="F35" s="68">
-        <f t="shared" ref="F35:F40" si="9">IF(ISBLANK(E35)," - ",IF(G35=0,E35,E35+G35-1))</f>
-        <v>43966</v>
+        <f t="shared" si="8"/>
+        <v>43973</v>
       </c>
       <c r="G35" s="52">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H35" s="53"/>
       <c r="I35" s="54"/>
@@ -6197,1217 +6193,18 @@
       <c r="BZ35" s="51"/>
       <c r="CA35" s="51"/>
     </row>
-    <row r="36" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A36" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>4.3</v>
-      </c>
-      <c r="B36" s="79" t="s">
-        <v>144</v>
-      </c>
-      <c r="C36" s="51"/>
-      <c r="D36" s="80"/>
-      <c r="E36" s="67">
-        <v>43962</v>
-      </c>
-      <c r="F36" s="68">
-        <f t="shared" si="9"/>
-        <v>43966</v>
-      </c>
-      <c r="G36" s="52">
-        <v>5</v>
-      </c>
-      <c r="H36" s="53"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="66"/>
-      <c r="K36" s="70"/>
-      <c r="L36" s="70"/>
-      <c r="M36" s="71"/>
-      <c r="N36" s="70"/>
-      <c r="O36" s="70"/>
-      <c r="P36" s="116"/>
-      <c r="Q36" s="116"/>
-      <c r="R36" s="70"/>
-      <c r="S36" s="70"/>
-      <c r="T36" s="70"/>
-      <c r="U36" s="70"/>
-      <c r="V36" s="70"/>
-      <c r="W36" s="116"/>
-      <c r="X36" s="116"/>
-      <c r="Y36" s="70"/>
-      <c r="Z36" s="70"/>
-      <c r="AA36" s="70"/>
-      <c r="AB36" s="70"/>
-      <c r="AC36" s="70"/>
-      <c r="AD36" s="116"/>
-      <c r="AE36" s="116"/>
-      <c r="AF36" s="70"/>
-      <c r="AG36" s="70"/>
-      <c r="AH36" s="70"/>
-      <c r="AI36" s="70"/>
-      <c r="AJ36" s="70"/>
-      <c r="AK36" s="116"/>
-      <c r="AL36" s="116"/>
-      <c r="AM36" s="70"/>
-      <c r="AN36" s="70"/>
-      <c r="AO36" s="70"/>
-      <c r="AP36" s="70"/>
-      <c r="AQ36" s="70"/>
-      <c r="AR36" s="116"/>
-      <c r="AS36" s="116"/>
-      <c r="AT36" s="70"/>
-      <c r="AU36" s="70"/>
-      <c r="AV36" s="70"/>
-      <c r="AW36" s="70"/>
-      <c r="AX36" s="70"/>
-      <c r="AY36" s="116"/>
-      <c r="AZ36" s="116"/>
-      <c r="BA36" s="70"/>
-      <c r="BB36" s="70"/>
-      <c r="BC36" s="70"/>
-      <c r="BD36" s="70"/>
-      <c r="BE36" s="70"/>
-      <c r="BF36" s="116"/>
-      <c r="BG36" s="116"/>
-      <c r="BH36" s="70"/>
-      <c r="BI36" s="70"/>
-      <c r="BJ36" s="70"/>
-      <c r="BK36" s="70"/>
-      <c r="BL36" s="70"/>
-      <c r="BM36" s="116"/>
-      <c r="BN36" s="116"/>
-      <c r="BO36" s="51"/>
-      <c r="BP36" s="51"/>
-      <c r="BQ36" s="51"/>
-      <c r="BR36" s="51"/>
-      <c r="BS36" s="51"/>
-      <c r="BT36" s="51"/>
-      <c r="BU36" s="51"/>
-      <c r="BV36" s="51"/>
-      <c r="BW36" s="51"/>
-      <c r="BX36" s="51"/>
-      <c r="BY36" s="51"/>
-      <c r="BZ36" s="51"/>
-      <c r="CA36" s="51"/>
-    </row>
-    <row r="37" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A37" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>4.4</v>
-      </c>
-      <c r="B37" s="79" t="s">
-        <v>135</v>
-      </c>
-      <c r="C37" s="51"/>
-      <c r="D37" s="80"/>
-      <c r="E37" s="67">
-        <v>43962</v>
-      </c>
-      <c r="F37" s="68">
-        <f t="shared" si="9"/>
-        <v>43966</v>
-      </c>
-      <c r="G37" s="52">
-        <v>5</v>
-      </c>
-      <c r="H37" s="53"/>
-      <c r="I37" s="54"/>
-      <c r="J37" s="66"/>
-      <c r="K37" s="70"/>
-      <c r="L37" s="70"/>
-      <c r="M37" s="70"/>
-      <c r="N37" s="70"/>
-      <c r="O37" s="70"/>
-      <c r="P37" s="116"/>
-      <c r="Q37" s="116"/>
-      <c r="R37" s="70"/>
-      <c r="S37" s="70"/>
-      <c r="T37" s="70"/>
-      <c r="U37" s="70"/>
-      <c r="V37" s="70"/>
-      <c r="W37" s="116"/>
-      <c r="X37" s="116"/>
-      <c r="Y37" s="70"/>
-      <c r="Z37" s="70"/>
-      <c r="AA37" s="70"/>
-      <c r="AB37" s="70"/>
-      <c r="AC37" s="70"/>
-      <c r="AD37" s="116"/>
-      <c r="AE37" s="116"/>
-      <c r="AF37" s="70"/>
-      <c r="AG37" s="70"/>
-      <c r="AH37" s="70"/>
-      <c r="AI37" s="70"/>
-      <c r="AJ37" s="70"/>
-      <c r="AK37" s="116"/>
-      <c r="AL37" s="116"/>
-      <c r="AM37" s="70"/>
-      <c r="AN37" s="70"/>
-      <c r="AO37" s="70"/>
-      <c r="AP37" s="70"/>
-      <c r="AQ37" s="70"/>
-      <c r="AR37" s="116"/>
-      <c r="AS37" s="116"/>
-      <c r="AT37" s="70"/>
-      <c r="AU37" s="70"/>
-      <c r="AV37" s="70"/>
-      <c r="AW37" s="70"/>
-      <c r="AX37" s="70"/>
-      <c r="AY37" s="116"/>
-      <c r="AZ37" s="116"/>
-      <c r="BA37" s="70"/>
-      <c r="BB37" s="70"/>
-      <c r="BC37" s="70"/>
-      <c r="BD37" s="70"/>
-      <c r="BE37" s="70"/>
-      <c r="BF37" s="116"/>
-      <c r="BG37" s="116"/>
-      <c r="BH37" s="70"/>
-      <c r="BI37" s="70"/>
-      <c r="BJ37" s="70"/>
-      <c r="BK37" s="70"/>
-      <c r="BL37" s="70"/>
-      <c r="BM37" s="116"/>
-      <c r="BN37" s="116"/>
-      <c r="BO37" s="51"/>
-      <c r="BP37" s="51"/>
-      <c r="BQ37" s="51"/>
-      <c r="BR37" s="51"/>
-      <c r="BS37" s="51"/>
-      <c r="BT37" s="51"/>
-      <c r="BU37" s="51"/>
-      <c r="BV37" s="51"/>
-      <c r="BW37" s="51"/>
-      <c r="BX37" s="51"/>
-      <c r="BY37" s="51"/>
-      <c r="BZ37" s="51"/>
-      <c r="CA37" s="51"/>
-    </row>
-    <row r="38" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A38" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
-      </c>
-      <c r="B38" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="51"/>
-      <c r="D38" s="80"/>
-      <c r="E38" s="67">
-        <v>43941</v>
-      </c>
-      <c r="F38" s="68">
-        <f t="shared" si="9"/>
-        <v>43941</v>
-      </c>
-      <c r="G38" s="52">
-        <v>1</v>
-      </c>
-      <c r="H38" s="53"/>
-      <c r="I38" s="54"/>
-      <c r="J38" s="66"/>
-      <c r="K38" s="70"/>
-      <c r="L38" s="70"/>
-      <c r="M38" s="70"/>
-      <c r="N38" s="70"/>
-      <c r="O38" s="70"/>
-      <c r="P38" s="116"/>
-      <c r="Q38" s="116"/>
-      <c r="R38" s="70"/>
-      <c r="S38" s="70"/>
-      <c r="T38" s="70"/>
-      <c r="U38" s="70"/>
-      <c r="V38" s="70"/>
-      <c r="W38" s="116"/>
-      <c r="X38" s="116"/>
-      <c r="Y38" s="70"/>
-      <c r="Z38" s="70"/>
-      <c r="AA38" s="70"/>
-      <c r="AB38" s="70"/>
-      <c r="AC38" s="70"/>
-      <c r="AD38" s="116"/>
-      <c r="AE38" s="116"/>
-      <c r="AF38" s="70"/>
-      <c r="AG38" s="70"/>
-      <c r="AH38" s="70"/>
-      <c r="AI38" s="70"/>
-      <c r="AJ38" s="70"/>
-      <c r="AK38" s="116"/>
-      <c r="AL38" s="116"/>
-      <c r="AM38" s="70"/>
-      <c r="AN38" s="70"/>
-      <c r="AO38" s="70"/>
-      <c r="AP38" s="70"/>
-      <c r="AQ38" s="70"/>
-      <c r="AR38" s="116"/>
-      <c r="AS38" s="116"/>
-      <c r="AT38" s="70"/>
-      <c r="AU38" s="70"/>
-      <c r="AV38" s="70"/>
-      <c r="AW38" s="70"/>
-      <c r="AX38" s="70"/>
-      <c r="AY38" s="116"/>
-      <c r="AZ38" s="116"/>
-      <c r="BA38" s="70"/>
-      <c r="BB38" s="70"/>
-      <c r="BC38" s="70"/>
-      <c r="BD38" s="70"/>
-      <c r="BE38" s="70"/>
-      <c r="BF38" s="116"/>
-      <c r="BG38" s="116"/>
-      <c r="BH38" s="70"/>
-      <c r="BI38" s="70"/>
-      <c r="BJ38" s="70"/>
-      <c r="BK38" s="70"/>
-      <c r="BL38" s="70"/>
-      <c r="BM38" s="116"/>
-      <c r="BN38" s="116"/>
-      <c r="BO38" s="51"/>
-      <c r="BP38" s="51"/>
-      <c r="BQ38" s="51"/>
-      <c r="BR38" s="51"/>
-      <c r="BS38" s="51"/>
-      <c r="BT38" s="51"/>
-      <c r="BU38" s="51"/>
-      <c r="BV38" s="51"/>
-      <c r="BW38" s="51"/>
-      <c r="BX38" s="51"/>
-      <c r="BY38" s="51"/>
-      <c r="BZ38" s="51"/>
-      <c r="CA38" s="51"/>
-    </row>
-    <row r="39" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A39" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>4.6</v>
-      </c>
-      <c r="B39" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="51"/>
-      <c r="D39" s="80"/>
-      <c r="E39" s="67">
-        <v>43941</v>
-      </c>
-      <c r="F39" s="68">
-        <f t="shared" si="9"/>
-        <v>43941</v>
-      </c>
-      <c r="G39" s="52">
-        <v>1</v>
-      </c>
-      <c r="H39" s="53"/>
-      <c r="I39" s="54"/>
-      <c r="J39" s="66"/>
-      <c r="K39" s="70"/>
-      <c r="L39" s="70"/>
-      <c r="M39" s="70"/>
-      <c r="N39" s="70"/>
-      <c r="O39" s="70"/>
-      <c r="P39" s="116"/>
-      <c r="Q39" s="116"/>
-      <c r="R39" s="70"/>
-      <c r="S39" s="70"/>
-      <c r="T39" s="70"/>
-      <c r="U39" s="70"/>
-      <c r="V39" s="70"/>
-      <c r="W39" s="116"/>
-      <c r="X39" s="116"/>
-      <c r="Y39" s="70"/>
-      <c r="Z39" s="70"/>
-      <c r="AA39" s="70"/>
-      <c r="AB39" s="70"/>
-      <c r="AC39" s="70"/>
-      <c r="AD39" s="116"/>
-      <c r="AE39" s="116"/>
-      <c r="AF39" s="70"/>
-      <c r="AG39" s="70"/>
-      <c r="AH39" s="70"/>
-      <c r="AI39" s="70"/>
-      <c r="AJ39" s="70"/>
-      <c r="AK39" s="116"/>
-      <c r="AL39" s="116"/>
-      <c r="AM39" s="70"/>
-      <c r="AN39" s="70"/>
-      <c r="AO39" s="70"/>
-      <c r="AP39" s="70"/>
-      <c r="AQ39" s="70"/>
-      <c r="AR39" s="116"/>
-      <c r="AS39" s="116"/>
-      <c r="AT39" s="70"/>
-      <c r="AU39" s="70"/>
-      <c r="AV39" s="70"/>
-      <c r="AW39" s="70"/>
-      <c r="AX39" s="70"/>
-      <c r="AY39" s="116"/>
-      <c r="AZ39" s="116"/>
-      <c r="BA39" s="70"/>
-      <c r="BB39" s="70"/>
-      <c r="BC39" s="70"/>
-      <c r="BD39" s="70"/>
-      <c r="BE39" s="70"/>
-      <c r="BF39" s="116"/>
-      <c r="BG39" s="116"/>
-      <c r="BH39" s="70"/>
-      <c r="BI39" s="70"/>
-      <c r="BJ39" s="70"/>
-      <c r="BK39" s="70"/>
-      <c r="BL39" s="70"/>
-      <c r="BM39" s="116"/>
-      <c r="BN39" s="116"/>
-      <c r="BO39" s="51"/>
-      <c r="BP39" s="51"/>
-      <c r="BQ39" s="51"/>
-      <c r="BR39" s="51"/>
-      <c r="BS39" s="51"/>
-      <c r="BT39" s="51"/>
-      <c r="BU39" s="51"/>
-      <c r="BV39" s="51"/>
-      <c r="BW39" s="51"/>
-      <c r="BX39" s="51"/>
-      <c r="BY39" s="51"/>
-      <c r="BZ39" s="51"/>
-      <c r="CA39" s="51"/>
-    </row>
-    <row r="40" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A40" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>4.7</v>
-      </c>
-      <c r="B40" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="51"/>
-      <c r="D40" s="80"/>
-      <c r="E40" s="67">
-        <v>43941</v>
-      </c>
-      <c r="F40" s="68">
-        <f t="shared" si="9"/>
-        <v>43941</v>
-      </c>
-      <c r="G40" s="52">
-        <v>1</v>
-      </c>
-      <c r="H40" s="53"/>
-      <c r="I40" s="54"/>
-      <c r="J40" s="66"/>
-      <c r="K40" s="70"/>
-      <c r="L40" s="70"/>
-      <c r="M40" s="70"/>
-      <c r="N40" s="70"/>
-      <c r="O40" s="70"/>
-      <c r="P40" s="116"/>
-      <c r="Q40" s="116"/>
-      <c r="R40" s="70"/>
-      <c r="S40" s="70"/>
-      <c r="T40" s="70"/>
-      <c r="U40" s="70"/>
-      <c r="V40" s="70"/>
-      <c r="W40" s="116"/>
-      <c r="X40" s="116"/>
-      <c r="Y40" s="70"/>
-      <c r="Z40" s="70"/>
-      <c r="AA40" s="70"/>
-      <c r="AB40" s="70"/>
-      <c r="AC40" s="70"/>
-      <c r="AD40" s="116"/>
-      <c r="AE40" s="116"/>
-      <c r="AF40" s="70"/>
-      <c r="AG40" s="70"/>
-      <c r="AH40" s="70"/>
-      <c r="AI40" s="70"/>
-      <c r="AJ40" s="70"/>
-      <c r="AK40" s="116"/>
-      <c r="AL40" s="116"/>
-      <c r="AM40" s="70"/>
-      <c r="AN40" s="70"/>
-      <c r="AO40" s="70"/>
-      <c r="AP40" s="70"/>
-      <c r="AQ40" s="70"/>
-      <c r="AR40" s="116"/>
-      <c r="AS40" s="116"/>
-      <c r="AT40" s="70"/>
-      <c r="AU40" s="70"/>
-      <c r="AV40" s="70"/>
-      <c r="AW40" s="70"/>
-      <c r="AX40" s="70"/>
-      <c r="AY40" s="116"/>
-      <c r="AZ40" s="116"/>
-      <c r="BA40" s="70"/>
-      <c r="BB40" s="70"/>
-      <c r="BC40" s="70"/>
-      <c r="BD40" s="70"/>
-      <c r="BE40" s="70"/>
-      <c r="BF40" s="116"/>
-      <c r="BG40" s="116"/>
-      <c r="BH40" s="70"/>
-      <c r="BI40" s="70"/>
-      <c r="BJ40" s="70"/>
-      <c r="BK40" s="70"/>
-      <c r="BL40" s="70"/>
-      <c r="BM40" s="116"/>
-      <c r="BN40" s="116"/>
-      <c r="BO40" s="51"/>
-      <c r="BP40" s="51"/>
-      <c r="BQ40" s="51"/>
-      <c r="BR40" s="51"/>
-      <c r="BS40" s="51"/>
-      <c r="BT40" s="51"/>
-      <c r="BU40" s="51"/>
-      <c r="BV40" s="51"/>
-      <c r="BW40" s="51"/>
-      <c r="BX40" s="51"/>
-      <c r="BY40" s="51"/>
-      <c r="BZ40" s="51"/>
-      <c r="CA40" s="51"/>
-    </row>
-    <row r="41" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A41" s="56" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>5</v>
-      </c>
-      <c r="B41" s="57" t="s">
-        <v>125</v>
-      </c>
-      <c r="C41" s="58"/>
-      <c r="D41" s="59"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="77" t="str">
-        <f>IF(ISBLANK(E41)," - ",IF(G41=0,E41,E41+G41-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G41" s="61"/>
-      <c r="H41" s="62"/>
-      <c r="I41" s="63" t="str">
-        <f>IF(OR(F41=0,E41=0)," - ",NETWORKDAYS(E41,F41))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J41" s="65"/>
-      <c r="K41" s="69"/>
-      <c r="L41" s="69"/>
-      <c r="M41" s="69"/>
-      <c r="N41" s="69"/>
-      <c r="O41" s="69"/>
-      <c r="P41" s="115"/>
-      <c r="Q41" s="115"/>
-      <c r="R41" s="69"/>
-      <c r="S41" s="69"/>
-      <c r="T41" s="69"/>
-      <c r="U41" s="69"/>
-      <c r="V41" s="69"/>
-      <c r="W41" s="115"/>
-      <c r="X41" s="115"/>
-      <c r="Y41" s="69"/>
-      <c r="Z41" s="69"/>
-      <c r="AA41" s="69"/>
-      <c r="AB41" s="69"/>
-      <c r="AC41" s="69"/>
-      <c r="AD41" s="115"/>
-      <c r="AE41" s="115"/>
-      <c r="AF41" s="69"/>
-      <c r="AG41" s="69"/>
-      <c r="AH41" s="69"/>
-      <c r="AI41" s="69"/>
-      <c r="AJ41" s="69"/>
-      <c r="AK41" s="115"/>
-      <c r="AL41" s="115"/>
-      <c r="AM41" s="69"/>
-      <c r="AN41" s="69"/>
-      <c r="AO41" s="69"/>
-      <c r="AP41" s="69"/>
-      <c r="AQ41" s="69"/>
-      <c r="AR41" s="115"/>
-      <c r="AS41" s="115"/>
-      <c r="AT41" s="69"/>
-      <c r="AU41" s="69"/>
-      <c r="AV41" s="69"/>
-      <c r="AW41" s="69"/>
-      <c r="AX41" s="69"/>
-      <c r="AY41" s="115"/>
-      <c r="AZ41" s="115"/>
-      <c r="BA41" s="69"/>
-      <c r="BB41" s="69"/>
-      <c r="BC41" s="69"/>
-      <c r="BD41" s="69"/>
-      <c r="BE41" s="69"/>
-      <c r="BF41" s="115"/>
-      <c r="BG41" s="115"/>
-      <c r="BH41" s="69"/>
-      <c r="BI41" s="69"/>
-      <c r="BJ41" s="69"/>
-      <c r="BK41" s="69"/>
-      <c r="BL41" s="69"/>
-      <c r="BM41" s="115"/>
-      <c r="BN41" s="115"/>
-      <c r="BO41" s="49"/>
-      <c r="BP41" s="49"/>
-      <c r="BQ41" s="49"/>
-      <c r="BR41" s="49"/>
-      <c r="BS41" s="49"/>
-      <c r="BT41" s="49"/>
-      <c r="BU41" s="49"/>
-      <c r="BV41" s="49"/>
-      <c r="BW41" s="49"/>
-      <c r="BX41" s="49"/>
-      <c r="BY41" s="49"/>
-      <c r="BZ41" s="49"/>
-      <c r="CA41" s="49"/>
-    </row>
-    <row r="42" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A42" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>5.1</v>
-      </c>
-      <c r="B42" s="79" t="s">
-        <v>148</v>
-      </c>
-      <c r="C42" s="51"/>
-      <c r="D42" s="80"/>
-      <c r="E42" s="67">
-        <v>43969</v>
-      </c>
-      <c r="F42" s="68">
-        <f>IF(ISBLANK(E42)," - ",IF(G42=0,E42,E42+G42-1))</f>
-        <v>43972</v>
-      </c>
-      <c r="G42" s="52">
-        <v>4</v>
-      </c>
-      <c r="H42" s="53"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="66"/>
-      <c r="K42" s="70"/>
-      <c r="L42" s="70"/>
-      <c r="M42" s="70"/>
-      <c r="N42" s="70"/>
-      <c r="O42" s="70"/>
-      <c r="P42" s="116"/>
-      <c r="Q42" s="116"/>
-      <c r="R42" s="70"/>
-      <c r="S42" s="70"/>
-      <c r="T42" s="70"/>
-      <c r="U42" s="70"/>
-      <c r="V42" s="70"/>
-      <c r="W42" s="116"/>
-      <c r="X42" s="116"/>
-      <c r="Y42" s="70"/>
-      <c r="Z42" s="70"/>
-      <c r="AA42" s="70"/>
-      <c r="AB42" s="70"/>
-      <c r="AC42" s="70"/>
-      <c r="AD42" s="116"/>
-      <c r="AE42" s="116"/>
-      <c r="AF42" s="70"/>
-      <c r="AG42" s="70"/>
-      <c r="AH42" s="70"/>
-      <c r="AI42" s="70"/>
-      <c r="AJ42" s="70"/>
-      <c r="AK42" s="116"/>
-      <c r="AL42" s="116"/>
-      <c r="AM42" s="70"/>
-      <c r="AN42" s="70"/>
-      <c r="AO42" s="70"/>
-      <c r="AP42" s="70"/>
-      <c r="AQ42" s="70"/>
-      <c r="AR42" s="116"/>
-      <c r="AS42" s="116"/>
-      <c r="AT42" s="70"/>
-      <c r="AU42" s="70"/>
-      <c r="AV42" s="70"/>
-      <c r="AW42" s="70"/>
-      <c r="AX42" s="70"/>
-      <c r="AY42" s="116"/>
-      <c r="AZ42" s="116"/>
-      <c r="BA42" s="70"/>
-      <c r="BB42" s="70"/>
-      <c r="BC42" s="70"/>
-      <c r="BD42" s="70"/>
-      <c r="BE42" s="70"/>
-      <c r="BF42" s="116"/>
-      <c r="BG42" s="116"/>
-      <c r="BH42" s="70"/>
-      <c r="BI42" s="70"/>
-      <c r="BJ42" s="70"/>
-      <c r="BK42" s="70"/>
-      <c r="BL42" s="70"/>
-      <c r="BM42" s="116"/>
-      <c r="BN42" s="116"/>
-      <c r="BO42" s="51"/>
-      <c r="BP42" s="51"/>
-      <c r="BQ42" s="51"/>
-      <c r="BR42" s="51"/>
-      <c r="BS42" s="51"/>
-      <c r="BT42" s="51"/>
-      <c r="BU42" s="51"/>
-      <c r="BV42" s="51"/>
-      <c r="BW42" s="51"/>
-      <c r="BX42" s="51"/>
-      <c r="BY42" s="51"/>
-      <c r="BZ42" s="51"/>
-      <c r="CA42" s="51"/>
-    </row>
-    <row r="43" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A43" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="B43" s="79" t="s">
-        <v>145</v>
-      </c>
-      <c r="C43" s="51"/>
-      <c r="D43" s="80"/>
-      <c r="E43" s="67">
-        <v>43969</v>
-      </c>
-      <c r="F43" s="68">
-        <f t="shared" ref="F43:F48" si="10">IF(ISBLANK(E43)," - ",IF(G43=0,E43,E43+G43-1))</f>
-        <v>43972</v>
-      </c>
-      <c r="G43" s="52">
-        <v>4</v>
-      </c>
-      <c r="H43" s="53"/>
-      <c r="I43" s="54"/>
-      <c r="J43" s="66"/>
-      <c r="K43" s="70"/>
-      <c r="L43" s="70"/>
-      <c r="M43" s="70"/>
-      <c r="N43" s="70"/>
-      <c r="O43" s="70"/>
-      <c r="P43" s="116"/>
-      <c r="Q43" s="116"/>
-      <c r="R43" s="70"/>
-      <c r="S43" s="70"/>
-      <c r="T43" s="70"/>
-      <c r="U43" s="70"/>
-      <c r="V43" s="70"/>
-      <c r="W43" s="116"/>
-      <c r="X43" s="116"/>
-      <c r="Y43" s="70"/>
-      <c r="Z43" s="70"/>
-      <c r="AA43" s="70"/>
-      <c r="AB43" s="70"/>
-      <c r="AC43" s="70"/>
-      <c r="AD43" s="116"/>
-      <c r="AE43" s="116"/>
-      <c r="AF43" s="70"/>
-      <c r="AG43" s="70"/>
-      <c r="AH43" s="70"/>
-      <c r="AI43" s="70"/>
-      <c r="AJ43" s="70"/>
-      <c r="AK43" s="116"/>
-      <c r="AL43" s="116"/>
-      <c r="AM43" s="70"/>
-      <c r="AN43" s="70"/>
-      <c r="AO43" s="70"/>
-      <c r="AP43" s="70"/>
-      <c r="AQ43" s="70"/>
-      <c r="AR43" s="116"/>
-      <c r="AS43" s="116"/>
-      <c r="AT43" s="70"/>
-      <c r="AU43" s="70"/>
-      <c r="AV43" s="70"/>
-      <c r="AW43" s="70"/>
-      <c r="AX43" s="70"/>
-      <c r="AY43" s="116"/>
-      <c r="AZ43" s="116"/>
-      <c r="BA43" s="70"/>
-      <c r="BB43" s="70"/>
-      <c r="BC43" s="70"/>
-      <c r="BD43" s="70"/>
-      <c r="BE43" s="70"/>
-      <c r="BF43" s="116"/>
-      <c r="BG43" s="116"/>
-      <c r="BH43" s="70"/>
-      <c r="BI43" s="70"/>
-      <c r="BJ43" s="70"/>
-      <c r="BK43" s="70"/>
-      <c r="BL43" s="70"/>
-      <c r="BM43" s="116"/>
-      <c r="BN43" s="116"/>
-      <c r="BO43" s="51"/>
-      <c r="BP43" s="51"/>
-      <c r="BQ43" s="51"/>
-      <c r="BR43" s="51"/>
-      <c r="BS43" s="51"/>
-      <c r="BT43" s="51"/>
-      <c r="BU43" s="51"/>
-      <c r="BV43" s="51"/>
-      <c r="BW43" s="51"/>
-      <c r="BX43" s="51"/>
-      <c r="BY43" s="51"/>
-      <c r="BZ43" s="51"/>
-      <c r="CA43" s="51"/>
-    </row>
-    <row r="44" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A44" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>5.3</v>
-      </c>
-      <c r="B44" s="79" t="s">
-        <v>146</v>
-      </c>
-      <c r="C44" s="51"/>
-      <c r="D44" s="80"/>
-      <c r="E44" s="67">
-        <v>43972</v>
-      </c>
-      <c r="F44" s="68">
-        <f t="shared" si="10"/>
-        <v>43973</v>
-      </c>
-      <c r="G44" s="52">
-        <v>2</v>
-      </c>
-      <c r="H44" s="53"/>
-      <c r="I44" s="54"/>
-      <c r="J44" s="66"/>
-      <c r="K44" s="70"/>
-      <c r="L44" s="70"/>
-      <c r="M44" s="71"/>
-      <c r="N44" s="70"/>
-      <c r="O44" s="70"/>
-      <c r="P44" s="116"/>
-      <c r="Q44" s="116"/>
-      <c r="R44" s="70"/>
-      <c r="S44" s="70"/>
-      <c r="T44" s="70"/>
-      <c r="U44" s="70"/>
-      <c r="V44" s="70"/>
-      <c r="W44" s="116"/>
-      <c r="X44" s="116"/>
-      <c r="Y44" s="70"/>
-      <c r="Z44" s="70"/>
-      <c r="AA44" s="70"/>
-      <c r="AB44" s="70"/>
-      <c r="AC44" s="70"/>
-      <c r="AD44" s="116"/>
-      <c r="AE44" s="116"/>
-      <c r="AF44" s="70"/>
-      <c r="AG44" s="70"/>
-      <c r="AH44" s="70"/>
-      <c r="AI44" s="70"/>
-      <c r="AJ44" s="70"/>
-      <c r="AK44" s="116"/>
-      <c r="AL44" s="116"/>
-      <c r="AM44" s="70"/>
-      <c r="AN44" s="70"/>
-      <c r="AO44" s="70"/>
-      <c r="AP44" s="70"/>
-      <c r="AQ44" s="70"/>
-      <c r="AR44" s="116"/>
-      <c r="AS44" s="116"/>
-      <c r="AT44" s="70"/>
-      <c r="AU44" s="70"/>
-      <c r="AV44" s="70"/>
-      <c r="AW44" s="70"/>
-      <c r="AX44" s="70"/>
-      <c r="AY44" s="116"/>
-      <c r="AZ44" s="116"/>
-      <c r="BA44" s="70"/>
-      <c r="BB44" s="70"/>
-      <c r="BC44" s="70"/>
-      <c r="BD44" s="70"/>
-      <c r="BE44" s="70"/>
-      <c r="BF44" s="116"/>
-      <c r="BG44" s="116"/>
-      <c r="BH44" s="70"/>
-      <c r="BI44" s="70"/>
-      <c r="BJ44" s="70"/>
-      <c r="BK44" s="70"/>
-      <c r="BL44" s="70"/>
-      <c r="BM44" s="116"/>
-      <c r="BN44" s="116"/>
-      <c r="BO44" s="51"/>
-      <c r="BP44" s="51"/>
-      <c r="BQ44" s="51"/>
-      <c r="BR44" s="51"/>
-      <c r="BS44" s="51"/>
-      <c r="BT44" s="51"/>
-      <c r="BU44" s="51"/>
-      <c r="BV44" s="51"/>
-      <c r="BW44" s="51"/>
-      <c r="BX44" s="51"/>
-      <c r="BY44" s="51"/>
-      <c r="BZ44" s="51"/>
-      <c r="CA44" s="51"/>
-    </row>
-    <row r="45" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A45" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>5.4</v>
-      </c>
-      <c r="B45" s="79" t="s">
-        <v>147</v>
-      </c>
-      <c r="C45" s="51"/>
-      <c r="D45" s="80"/>
-      <c r="E45" s="67">
-        <v>43973</v>
-      </c>
-      <c r="F45" s="68">
-        <f t="shared" si="10"/>
-        <v>43973</v>
-      </c>
-      <c r="G45" s="52">
-        <v>1</v>
-      </c>
-      <c r="H45" s="53"/>
-      <c r="I45" s="54"/>
-      <c r="J45" s="66"/>
-      <c r="K45" s="70"/>
-      <c r="L45" s="70"/>
-      <c r="M45" s="70"/>
-      <c r="N45" s="70"/>
-      <c r="O45" s="70"/>
-      <c r="P45" s="116"/>
-      <c r="Q45" s="116"/>
-      <c r="R45" s="70"/>
-      <c r="S45" s="70"/>
-      <c r="T45" s="70"/>
-      <c r="U45" s="70"/>
-      <c r="V45" s="70"/>
-      <c r="W45" s="116"/>
-      <c r="X45" s="116"/>
-      <c r="Y45" s="70"/>
-      <c r="Z45" s="70"/>
-      <c r="AA45" s="70"/>
-      <c r="AB45" s="70"/>
-      <c r="AC45" s="70"/>
-      <c r="AD45" s="116"/>
-      <c r="AE45" s="116"/>
-      <c r="AF45" s="70"/>
-      <c r="AG45" s="70"/>
-      <c r="AH45" s="70"/>
-      <c r="AI45" s="70"/>
-      <c r="AJ45" s="70"/>
-      <c r="AK45" s="116"/>
-      <c r="AL45" s="116"/>
-      <c r="AM45" s="70"/>
-      <c r="AN45" s="70"/>
-      <c r="AO45" s="70"/>
-      <c r="AP45" s="70"/>
-      <c r="AQ45" s="70"/>
-      <c r="AR45" s="116"/>
-      <c r="AS45" s="116"/>
-      <c r="AT45" s="70"/>
-      <c r="AU45" s="70"/>
-      <c r="AV45" s="70"/>
-      <c r="AW45" s="70"/>
-      <c r="AX45" s="70"/>
-      <c r="AY45" s="116"/>
-      <c r="AZ45" s="116"/>
-      <c r="BA45" s="70"/>
-      <c r="BB45" s="70"/>
-      <c r="BC45" s="70"/>
-      <c r="BD45" s="70"/>
-      <c r="BE45" s="70"/>
-      <c r="BF45" s="116"/>
-      <c r="BG45" s="116"/>
-      <c r="BH45" s="70"/>
-      <c r="BI45" s="70"/>
-      <c r="BJ45" s="70"/>
-      <c r="BK45" s="70"/>
-      <c r="BL45" s="70"/>
-      <c r="BM45" s="116"/>
-      <c r="BN45" s="116"/>
-      <c r="BO45" s="51"/>
-      <c r="BP45" s="51"/>
-      <c r="BQ45" s="51"/>
-      <c r="BR45" s="51"/>
-      <c r="BS45" s="51"/>
-      <c r="BT45" s="51"/>
-      <c r="BU45" s="51"/>
-      <c r="BV45" s="51"/>
-      <c r="BW45" s="51"/>
-      <c r="BX45" s="51"/>
-      <c r="BY45" s="51"/>
-      <c r="BZ45" s="51"/>
-      <c r="CA45" s="51"/>
-    </row>
-    <row r="46" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A46" s="50" t="str">
-        <f t="shared" si="6"/>
-        <v>5.5</v>
-      </c>
-      <c r="B46" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="51"/>
-      <c r="D46" s="80"/>
-      <c r="E46" s="67">
-        <v>43941</v>
-      </c>
-      <c r="F46" s="68">
-        <f t="shared" si="10"/>
-        <v>43941</v>
-      </c>
-      <c r="G46" s="52">
-        <v>1</v>
-      </c>
-      <c r="H46" s="53"/>
-      <c r="I46" s="54"/>
-      <c r="J46" s="66"/>
-      <c r="K46" s="70"/>
-      <c r="L46" s="70"/>
-      <c r="M46" s="70"/>
-      <c r="N46" s="70"/>
-      <c r="O46" s="70"/>
-      <c r="P46" s="116"/>
-      <c r="Q46" s="116"/>
-      <c r="R46" s="70"/>
-      <c r="S46" s="70"/>
-      <c r="T46" s="70"/>
-      <c r="U46" s="70"/>
-      <c r="V46" s="70"/>
-      <c r="W46" s="116"/>
-      <c r="X46" s="116"/>
-      <c r="Y46" s="70"/>
-      <c r="Z46" s="70"/>
-      <c r="AA46" s="70"/>
-      <c r="AB46" s="70"/>
-      <c r="AC46" s="70"/>
-      <c r="AD46" s="116"/>
-      <c r="AE46" s="116"/>
-      <c r="AF46" s="70"/>
-      <c r="AG46" s="70"/>
-      <c r="AH46" s="70"/>
-      <c r="AI46" s="70"/>
-      <c r="AJ46" s="70"/>
-      <c r="AK46" s="116"/>
-      <c r="AL46" s="116"/>
-      <c r="AM46" s="70"/>
-      <c r="AN46" s="70"/>
-      <c r="AO46" s="70"/>
-      <c r="AP46" s="70"/>
-      <c r="AQ46" s="70"/>
-      <c r="AR46" s="116"/>
-      <c r="AS46" s="116"/>
-      <c r="AT46" s="70"/>
-      <c r="AU46" s="70"/>
-      <c r="AV46" s="70"/>
-      <c r="AW46" s="70"/>
-      <c r="AX46" s="70"/>
-      <c r="AY46" s="116"/>
-      <c r="AZ46" s="116"/>
-      <c r="BA46" s="70"/>
-      <c r="BB46" s="70"/>
-      <c r="BC46" s="70"/>
-      <c r="BD46" s="70"/>
-      <c r="BE46" s="70"/>
-      <c r="BF46" s="116"/>
-      <c r="BG46" s="116"/>
-      <c r="BH46" s="70"/>
-      <c r="BI46" s="70"/>
-      <c r="BJ46" s="70"/>
-      <c r="BK46" s="70"/>
-      <c r="BL46" s="70"/>
-      <c r="BM46" s="116"/>
-      <c r="BN46" s="116"/>
-      <c r="BO46" s="51"/>
-      <c r="BP46" s="51"/>
-      <c r="BQ46" s="51"/>
-      <c r="BR46" s="51"/>
-      <c r="BS46" s="51"/>
-      <c r="BT46" s="51"/>
-      <c r="BU46" s="51"/>
-      <c r="BV46" s="51"/>
-      <c r="BW46" s="51"/>
-      <c r="BX46" s="51"/>
-      <c r="BY46" s="51"/>
-      <c r="BZ46" s="51"/>
-      <c r="CA46" s="51"/>
-    </row>
-    <row r="47" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A47" s="50" t="str">
-        <f t="shared" ref="A47:A48" si="11">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.6</v>
-      </c>
-      <c r="B47" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" s="51"/>
-      <c r="D47" s="80"/>
-      <c r="E47" s="67">
-        <v>43941</v>
-      </c>
-      <c r="F47" s="68">
-        <f t="shared" si="10"/>
-        <v>43941</v>
-      </c>
-      <c r="G47" s="52">
-        <v>1</v>
-      </c>
-      <c r="H47" s="53"/>
-      <c r="I47" s="54"/>
-      <c r="J47" s="66"/>
-      <c r="K47" s="70"/>
-      <c r="L47" s="70"/>
-      <c r="M47" s="70"/>
-      <c r="N47" s="70"/>
-      <c r="O47" s="70"/>
-      <c r="P47" s="116"/>
-      <c r="Q47" s="116"/>
-      <c r="R47" s="70"/>
-      <c r="S47" s="70"/>
-      <c r="T47" s="70"/>
-      <c r="U47" s="70"/>
-      <c r="V47" s="70"/>
-      <c r="W47" s="116"/>
-      <c r="X47" s="116"/>
-      <c r="Y47" s="70"/>
-      <c r="Z47" s="70"/>
-      <c r="AA47" s="70"/>
-      <c r="AB47" s="70"/>
-      <c r="AC47" s="70"/>
-      <c r="AD47" s="116"/>
-      <c r="AE47" s="116"/>
-      <c r="AF47" s="70"/>
-      <c r="AG47" s="70"/>
-      <c r="AH47" s="70"/>
-      <c r="AI47" s="70"/>
-      <c r="AJ47" s="70"/>
-      <c r="AK47" s="116"/>
-      <c r="AL47" s="116"/>
-      <c r="AM47" s="70"/>
-      <c r="AN47" s="70"/>
-      <c r="AO47" s="70"/>
-      <c r="AP47" s="70"/>
-      <c r="AQ47" s="70"/>
-      <c r="AR47" s="116"/>
-      <c r="AS47" s="116"/>
-      <c r="AT47" s="70"/>
-      <c r="AU47" s="70"/>
-      <c r="AV47" s="70"/>
-      <c r="AW47" s="70"/>
-      <c r="AX47" s="70"/>
-      <c r="AY47" s="116"/>
-      <c r="AZ47" s="116"/>
-      <c r="BA47" s="70"/>
-      <c r="BB47" s="70"/>
-      <c r="BC47" s="70"/>
-      <c r="BD47" s="70"/>
-      <c r="BE47" s="70"/>
-      <c r="BF47" s="116"/>
-      <c r="BG47" s="116"/>
-      <c r="BH47" s="70"/>
-      <c r="BI47" s="70"/>
-      <c r="BJ47" s="70"/>
-      <c r="BK47" s="70"/>
-      <c r="BL47" s="70"/>
-      <c r="BM47" s="116"/>
-      <c r="BN47" s="116"/>
-      <c r="BO47" s="51"/>
-      <c r="BP47" s="51"/>
-      <c r="BQ47" s="51"/>
-      <c r="BR47" s="51"/>
-      <c r="BS47" s="51"/>
-      <c r="BT47" s="51"/>
-      <c r="BU47" s="51"/>
-      <c r="BV47" s="51"/>
-      <c r="BW47" s="51"/>
-      <c r="BX47" s="51"/>
-      <c r="BY47" s="51"/>
-      <c r="BZ47" s="51"/>
-      <c r="CA47" s="51"/>
-    </row>
-    <row r="48" spans="1:79" ht="18" x14ac:dyDescent="0.15">
-      <c r="A48" s="50" t="str">
-        <f t="shared" si="11"/>
-        <v>5.7</v>
-      </c>
-      <c r="B48" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" s="51"/>
-      <c r="D48" s="80"/>
-      <c r="E48" s="67">
-        <v>43941</v>
-      </c>
-      <c r="F48" s="68">
-        <f t="shared" si="10"/>
-        <v>43941</v>
-      </c>
-      <c r="G48" s="52">
-        <v>1</v>
-      </c>
-      <c r="H48" s="53"/>
-      <c r="I48" s="54"/>
-      <c r="J48" s="66"/>
-      <c r="K48" s="70"/>
-      <c r="L48" s="70"/>
-      <c r="M48" s="70"/>
-      <c r="N48" s="70"/>
-      <c r="O48" s="70"/>
-      <c r="P48" s="116"/>
-      <c r="Q48" s="116"/>
-      <c r="R48" s="70"/>
-      <c r="S48" s="70"/>
-      <c r="T48" s="70"/>
-      <c r="U48" s="70"/>
-      <c r="V48" s="70"/>
-      <c r="W48" s="116"/>
-      <c r="X48" s="116"/>
-      <c r="Y48" s="70"/>
-      <c r="Z48" s="70"/>
-      <c r="AA48" s="70"/>
-      <c r="AB48" s="70"/>
-      <c r="AC48" s="70"/>
-      <c r="AD48" s="116"/>
-      <c r="AE48" s="116"/>
-      <c r="AF48" s="70"/>
-      <c r="AG48" s="70"/>
-      <c r="AH48" s="70"/>
-      <c r="AI48" s="70"/>
-      <c r="AJ48" s="70"/>
-      <c r="AK48" s="116"/>
-      <c r="AL48" s="116"/>
-      <c r="AM48" s="70"/>
-      <c r="AN48" s="70"/>
-      <c r="AO48" s="70"/>
-      <c r="AP48" s="70"/>
-      <c r="AQ48" s="70"/>
-      <c r="AR48" s="116"/>
-      <c r="AS48" s="116"/>
-      <c r="AT48" s="70"/>
-      <c r="AU48" s="70"/>
-      <c r="AV48" s="70"/>
-      <c r="AW48" s="70"/>
-      <c r="AX48" s="70"/>
-      <c r="AY48" s="116"/>
-      <c r="AZ48" s="116"/>
-      <c r="BA48" s="70"/>
-      <c r="BB48" s="70"/>
-      <c r="BC48" s="70"/>
-      <c r="BD48" s="70"/>
-      <c r="BE48" s="70"/>
-      <c r="BF48" s="116"/>
-      <c r="BG48" s="116"/>
-      <c r="BH48" s="70"/>
-      <c r="BI48" s="70"/>
-      <c r="BJ48" s="70"/>
-      <c r="BK48" s="70"/>
-      <c r="BL48" s="70"/>
-      <c r="BM48" s="116"/>
-      <c r="BN48" s="116"/>
-      <c r="BO48" s="51"/>
-      <c r="BP48" s="51"/>
-      <c r="BQ48" s="51"/>
-      <c r="BR48" s="51"/>
-      <c r="BS48" s="51"/>
-      <c r="BT48" s="51"/>
-      <c r="BU48" s="51"/>
-      <c r="BV48" s="51"/>
-      <c r="BW48" s="51"/>
-      <c r="BX48" s="51"/>
-      <c r="BY48" s="51"/>
-      <c r="BZ48" s="51"/>
-      <c r="CA48" s="51"/>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -7418,18 +6215,9 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H7:H48">
+  <conditionalFormatting sqref="H7:H35">
     <cfRule type="dataBar" priority="46">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -7448,7 +6236,7 @@
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7:BN48">
+  <conditionalFormatting sqref="K7:BN35">
     <cfRule type="expression" dxfId="2" priority="92">
       <formula>AND($E7&lt;=K$6,ROUNDDOWN(($F7-$E7+1)*$H7,0)+$E7-1&gt;=K$6)</formula>
     </cfRule>
@@ -7456,7 +6244,7 @@
       <formula>AND(NOT(ISBLANK($E7)),$E7&lt;=K$6,$F7&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN48">
+  <conditionalFormatting sqref="K6:BN35">
     <cfRule type="expression" dxfId="0" priority="52">
       <formula>K$6=TODAY()</formula>
     </cfRule>
@@ -7513,7 +6301,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H7:H48</xm:sqref>
+          <xm:sqref>H7:H35</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -7542,17 +6330,17 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C4" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C5" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
@@ -7560,149 +6348,149 @@
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C7" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C8" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C10" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C11" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C13" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B19" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B20" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="2:2" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B22" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B23" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B24" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="2:2" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B26" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B27" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B28" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B29" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B30" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B31" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B32" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B34" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B35" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B36" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B37" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B39" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B40" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="2:2" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B42" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B43" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B44" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="46" spans="2:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B46" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -7712,7 +6500,7 @@
     <hyperlink ref="C13" r:id="rId3" display="https://www.vertex42.com/blog/business/pm/new-gantt-chart-for-excel-online.html" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="93" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId4"/>
   <drawing r:id="rId5"/>
 </worksheet>
 </file>
@@ -7736,14 +6524,14 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="38"/>
     </row>
     <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="88" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="8"/>
@@ -7755,28 +6543,28 @@
     </row>
     <row r="4" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="83" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="35"/>
     </row>
     <row r="5" spans="1:3" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="B5" s="89" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="B7" s="89" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="B9" s="88" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="B11" s="87" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.15"/>
@@ -7790,13 +6578,13 @@
     <row r="15" spans="1:3" s="84" customFormat="1" ht="18" x14ac:dyDescent="0.15">
       <c r="A15" s="92"/>
       <c r="B15" s="90" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="84" customFormat="1" ht="18" x14ac:dyDescent="0.15">
       <c r="A16" s="92"/>
       <c r="B16" s="91" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="86" t="s">
         <v>1</v>
@@ -7805,25 +6593,25 @@
     <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="93"/>
       <c r="B17" s="91" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="93"/>
       <c r="B18" s="91" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="38" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="96"/>
       <c r="B19" s="91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="84" customFormat="1" ht="18" x14ac:dyDescent="0.15">
       <c r="A20" s="92"/>
       <c r="B20" s="90" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="85" t="s">
         <v>0</v>
@@ -7832,13 +6620,13 @@
     <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="93"/>
       <c r="B21" s="91" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="94"/>
       <c r="B22" s="95" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -7847,14 +6635,14 @@
     </row>
     <row r="24" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="126" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" s="126"/>
     </row>
     <row r="25" spans="1:3" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" s="94"/>
       <c r="B25" s="91" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -7864,19 +6652,19 @@
     <row r="27" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="94"/>
       <c r="B27" s="112" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="94"/>
       <c r="B28" s="91" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="94"/>
       <c r="B29" s="91" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -7886,19 +6674,19 @@
     <row r="31" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="94"/>
       <c r="B31" s="112" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="94"/>
       <c r="B32" s="91" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="94"/>
       <c r="B33" s="91" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -7908,13 +6696,13 @@
     <row r="35" spans="1:2" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="94"/>
       <c r="B35" s="91" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="94"/>
       <c r="B36" s="97" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -7923,31 +6711,31 @@
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="126" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" s="126"/>
     </row>
     <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.15">
       <c r="B39" s="91" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="41" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="B41" s="91" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="43" spans="1:2" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="B43" s="91" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.15">
       <c r="B45" s="91" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
@@ -7955,7 +6743,7 @@
     </row>
     <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.15">
       <c r="B47" s="91" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
@@ -7969,7 +6757,7 @@
     </row>
     <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.15">
       <c r="B50" s="91" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
@@ -7977,86 +6765,86 @@
     </row>
     <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A52" s="98" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="91" t="s">
         <v>9</v>
-      </c>
-      <c r="B52" s="91" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A53" s="98" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="91" t="s">
         <v>11</v>
-      </c>
-      <c r="B53" s="91" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A54" s="98" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="91" t="s">
         <v>13</v>
-      </c>
-      <c r="B54" s="91" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="30" x14ac:dyDescent="0.15">
       <c r="A55" s="87"/>
       <c r="B55" s="91" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="30" x14ac:dyDescent="0.15">
       <c r="A56" s="87"/>
       <c r="B56" s="91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A57" s="98" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="91" t="s">
         <v>15</v>
-      </c>
-      <c r="B57" s="91" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A58" s="87"/>
       <c r="B58" s="91" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A59" s="87"/>
       <c r="B59" s="91" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A60" s="98" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" s="91" t="s">
         <v>17</v>
-      </c>
-      <c r="B60" s="91" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="30" x14ac:dyDescent="0.15">
       <c r="A61" s="87"/>
       <c r="B61" s="91" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A62" s="98" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" s="91" t="s">
         <v>93</v>
-      </c>
-      <c r="B62" s="91" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A63" s="99"/>
       <c r="B63" s="91" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.15">
@@ -8064,13 +6852,13 @@
     </row>
     <row r="65" spans="1:2" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="126" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B65" s="126"/>
     </row>
     <row r="66" spans="1:2" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="B66" s="91" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.15">
@@ -8087,13 +6875,13 @@
         <v>4</v>
       </c>
       <c r="B69" s="107" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:2" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A70" s="100"/>
       <c r="B70" s="105" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="71" spans="1:2" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.15">
@@ -8105,13 +6893,13 @@
         <v>4</v>
       </c>
       <c r="B72" s="107" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:2" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A73" s="100"/>
       <c r="B73" s="105" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:2" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.15">
@@ -8123,13 +6911,13 @@
         <v>4</v>
       </c>
       <c r="B75" s="109" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="76" spans="1:2" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A76" s="100"/>
       <c r="B76" s="89" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="14" x14ac:dyDescent="0.15">
@@ -8141,13 +6929,13 @@
         <v>4</v>
       </c>
       <c r="B78" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="79" spans="1:2" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A79" s="100"/>
       <c r="B79" s="89" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80" spans="1:2" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
@@ -8159,25 +6947,25 @@
         <v>4</v>
       </c>
       <c r="B81" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="82" spans="1:2" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A82" s="100"/>
       <c r="B82" s="104" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:2" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A83" s="100"/>
       <c r="B83" s="104" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:2" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A84" s="100"/>
       <c r="B84" s="104" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14" x14ac:dyDescent="0.15">
@@ -8189,25 +6977,25 @@
         <v>4</v>
       </c>
       <c r="B86" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="87" spans="1:2" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A87" s="100"/>
       <c r="B87" s="89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="88" spans="1:2" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A88" s="100"/>
       <c r="B88" s="102" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="1:2" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A89" s="100"/>
       <c r="B89" s="108" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14" x14ac:dyDescent="0.15">
@@ -8219,18 +7007,18 @@
         <v>4</v>
       </c>
       <c r="B91" s="111" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="30" x14ac:dyDescent="0.15">
       <c r="A92" s="87"/>
       <c r="B92" s="104" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A94" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -8249,7 +7037,7 @@
     <hyperlink ref="B36" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.25" bottom="0.25" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId5"/>
   <legacyDrawing r:id="rId6"/>
@@ -8273,7 +7061,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="41"/>
@@ -8288,14 +7076,14 @@
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
       <c r="B3" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="40"/>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="14"/>
       <c r="B4" s="34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="15"/>
     </row>
@@ -8307,7 +7095,7 @@
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="15"/>
     </row>
@@ -8319,7 +7107,7 @@
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="15"/>
     </row>
@@ -8331,7 +7119,7 @@
     <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="14"/>
       <c r="B10" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="15"/>
     </row>
@@ -8343,7 +7131,7 @@
     <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
       <c r="B12" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="15"/>
     </row>
@@ -8355,7 +7143,7 @@
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
       <c r="B14" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="15"/>
     </row>
@@ -8367,7 +7155,7 @@
     <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="15"/>
     </row>
@@ -8379,14 +7167,14 @@
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="15"/>
     </row>
     <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="15"/>
     </row>
@@ -8446,7 +7234,7 @@
     <hyperlink ref="B19" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>